<commit_message>
Fix spelling error in std naming
</commit_message>
<xml_diff>
--- a/inst/resources/bam_var_names.xlsx
+++ b/inst/resources/bam_var_names.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samantha.schiano\Documents\GitHub-Repos\asar\inst\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094A9C9B-1F21-4F50-8EB8-D1242B8E0A0B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB0D974-E2AC-4A91-A95D-DA5509C3DBF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10404" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="374">
   <si>
     <t>label</t>
   </si>
@@ -1139,6 +1139,9 @@
   </si>
   <si>
     <t>projected_abundance</t>
+  </si>
+  <si>
+    <t>log_recruitment_deviations</t>
   </si>
 </sst>
 </file>
@@ -1411,8 +1414,8 @@
   </sheetPr>
   <dimension ref="A1:B267"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="B176" sqref="B176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2660,7 +2663,7 @@
         <v>252</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>189</v>
+        <v>373</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update(BAM fleet names): add another param to extract fleet names
Also change translated naming sheet - repeated label
</commit_message>
<xml_diff>
--- a/inst/resources/bam_var_names.xlsx
+++ b/inst/resources/bam_var_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samantha.schiano\Documents\GitHub-Repos\asar\inst\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B415980-1889-4528-B410-4050CA4FABD5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C32A076-F542-4B00-B7CD-2899A4A7399D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10404" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="375">
   <si>
     <t>label</t>
   </si>
@@ -1488,10 +1488,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B268"/>
+  <dimension ref="A1:B267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="B247" sqref="B247"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1548,79 +1548,81 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>11</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>365</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>23</v>
@@ -1628,7 +1630,7 @@
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>23</v>
@@ -1636,7 +1638,7 @@
     </row>
     <row r="19" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>23</v>
@@ -1644,7 +1646,7 @@
     </row>
     <row r="20" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>23</v>
@@ -1652,43 +1654,43 @@
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B23" s="3"/>
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B24" s="3"/>
     </row>
     <row r="25" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>366</v>
@@ -1696,7 +1698,7 @@
     </row>
     <row r="27" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>366</v>
@@ -1704,7 +1706,7 @@
     </row>
     <row r="28" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>366</v>
@@ -1712,1720 +1714,1712 @@
     </row>
     <row r="29" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>56</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="B39" s="3"/>
     </row>
     <row r="40" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B41" s="3"/>
     </row>
     <row r="42" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B42" s="3"/>
-    </row>
-    <row r="43" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>123</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>54</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="B44" s="3"/>
     </row>
     <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B45" s="3"/>
     </row>
     <row r="46" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B46" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="47" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>370</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>88</v>
+        <v>371</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>23</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="B68" s="3"/>
     </row>
     <row r="69" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B69" s="3"/>
     </row>
     <row r="70" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B70" s="3"/>
-    </row>
-    <row r="71" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>113</v>
+        <v>13</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>114</v>
+        <v>13</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="B78" s="3"/>
     </row>
     <row r="79" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B79" s="3"/>
+        <v>116</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="80" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>123</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="B83" s="3"/>
     </row>
     <row r="84" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B84" s="3"/>
     </row>
     <row r="85" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B85" s="3"/>
     </row>
-    <row r="86" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B86" s="3"/>
-    </row>
-    <row r="87" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="6" t="s">
+    <row r="86" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="B87" s="7"/>
+      <c r="B86" s="7"/>
+    </row>
+    <row r="87" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B87" s="3"/>
     </row>
     <row r="88" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B88" s="3"/>
     </row>
-    <row r="89" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B89" s="3"/>
-    </row>
-    <row r="90" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>9</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="B96" s="3"/>
     </row>
     <row r="97" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B97" s="3"/>
     </row>
     <row r="98" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B98" s="3"/>
     </row>
     <row r="99" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B99" s="3"/>
     </row>
     <row r="100" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B100" s="3"/>
-    </row>
-    <row r="101" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>372</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="B101" s="3"/>
     </row>
     <row r="102" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B102" s="3"/>
     </row>
     <row r="103" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B103" s="3"/>
     </row>
     <row r="104" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B104" s="3"/>
     </row>
     <row r="105" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B105" s="3"/>
     </row>
     <row r="106" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B106" s="3"/>
     </row>
     <row r="107" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B107" s="3"/>
     </row>
     <row r="108" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B108" s="3"/>
     </row>
     <row r="109" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B109" s="3"/>
     </row>
     <row r="110" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B110" s="3"/>
     </row>
-    <row r="111" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="2" t="s">
-        <v>158</v>
+    <row r="111" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="5" t="s">
+        <v>159</v>
       </c>
       <c r="B111" s="3"/>
     </row>
-    <row r="112" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="5" t="s">
-        <v>159</v>
+    <row r="112" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="2" t="s">
+        <v>160</v>
       </c>
       <c r="B112" s="3"/>
     </row>
     <row r="113" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B113" s="3"/>
     </row>
     <row r="114" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B114" s="3"/>
     </row>
     <row r="115" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B115" s="3"/>
-    </row>
-    <row r="116" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>264</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="B117" s="3"/>
     </row>
     <row r="118" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B118" s="3"/>
     </row>
     <row r="119" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B119" s="3"/>
     </row>
     <row r="120" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B120" s="3"/>
     </row>
     <row r="121" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B121" s="3"/>
     </row>
     <row r="122" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B122" s="3"/>
     </row>
     <row r="123" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B123" s="3"/>
     </row>
     <row r="124" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B124" s="3"/>
     </row>
     <row r="125" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B125" s="3"/>
     </row>
     <row r="126" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B126" s="3"/>
-    </row>
-    <row r="127" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>187</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="B133" s="3"/>
     </row>
     <row r="134" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B134" s="3"/>
     </row>
     <row r="135" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B135" s="3"/>
-    </row>
-    <row r="136" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>191</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="B136" s="3"/>
     </row>
     <row r="137" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B137" s="3"/>
+        <v>193</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="138" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>198</v>
+        <v>42</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="B146" s="2" t="s">
-        <v>209</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="B146" s="3"/>
     </row>
     <row r="147" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B147" s="3"/>
     </row>
     <row r="148" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B148" s="3"/>
     </row>
     <row r="149" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B149" s="3"/>
+        <v>213</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="150" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="B150" s="2" t="s">
-        <v>214</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="B150" s="3"/>
     </row>
     <row r="151" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B151" s="3"/>
     </row>
     <row r="152" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B152" s="3"/>
     </row>
     <row r="153" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B153" s="3"/>
     </row>
     <row r="154" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B154" s="3"/>
     </row>
     <row r="155" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B155" s="3"/>
     </row>
-    <row r="156" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B156" s="3"/>
     </row>
     <row r="157" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B157" s="3"/>
     </row>
     <row r="158" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B158" s="3"/>
     </row>
     <row r="159" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B159" s="3"/>
     </row>
     <row r="160" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B160" s="3"/>
-    </row>
-    <row r="161" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="2" t="s">
         <v>225</v>
       </c>
+      <c r="B160" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A161" s="5" t="s">
+        <v>227</v>
+      </c>
       <c r="B161" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="5" t="s">
-        <v>227</v>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A162" s="2" t="s">
+        <v>229</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A163" s="5" t="s">
+        <v>231</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="5" t="s">
-        <v>231</v>
+        <v>232</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A164" s="2" t="s">
+        <v>233</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A165" s="5" t="s">
+        <v>235</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A166" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="B166" s="2" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A166" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B166" s="3"/>
+    </row>
+    <row r="167" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B167" s="3"/>
     </row>
-    <row r="168" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B168" s="3"/>
     </row>
     <row r="169" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="B169" s="3"/>
+        <v>240</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="170" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>201</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="B172" s="3"/>
     </row>
     <row r="173" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="B173" s="3"/>
-    </row>
-    <row r="174" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>244</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>374</v>
+        <v>194</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>194</v>
+        <v>54</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>361</v>
+        <v>249</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="B182" s="2" t="s">
-        <v>257</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="B182" s="3"/>
     </row>
     <row r="183" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="B183" s="3"/>
-    </row>
-    <row r="184" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A188" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A188" s="5" t="s">
+        <v>269</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A189" s="5" t="s">
-        <v>269</v>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A189" s="2" t="s">
+        <v>271</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="B191" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>274</v>
+      </c>
+      <c r="B191" s="3"/>
     </row>
     <row r="192" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B192" s="3"/>
     </row>
     <row r="193" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B193" s="3"/>
     </row>
     <row r="194" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="B194" s="3"/>
-    </row>
-    <row r="195" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A195" s="2" t="s">
         <v>277</v>
       </c>
+      <c r="B194" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A195" s="5" t="s">
+        <v>279</v>
+      </c>
       <c r="B195" s="2" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="5" t="s">
-        <v>279</v>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A196" s="2" t="s">
+        <v>281</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A198" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A198" s="5" t="s">
+        <v>285</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A199" s="5" t="s">
-        <v>285</v>
+        <v>286</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A199" s="2" t="s">
+        <v>287</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="B200" s="2" t="s">
-        <v>288</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="B200" s="3"/>
     </row>
     <row r="201" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B201" s="3"/>
     </row>
-    <row r="202" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A202" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B202" s="3"/>
     </row>
-    <row r="203" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A203" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="B203" s="3"/>
-    </row>
-    <row r="204" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A204" s="6" t="s">
+    <row r="203" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A203" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B204" s="7"/>
+      <c r="B203" s="7"/>
+    </row>
+    <row r="204" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A204" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B204" s="3"/>
     </row>
     <row r="205" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B205" s="3"/>
     </row>
-    <row r="206" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B206" s="3"/>
     </row>
     <row r="207" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A207" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B207" s="3"/>
     </row>
     <row r="208" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B208" s="3"/>
     </row>
     <row r="209" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A209" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B209" s="3"/>
     </row>
-    <row r="210" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B210" s="3"/>
     </row>
     <row r="211" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B211" s="3"/>
     </row>
     <row r="212" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B212" s="3"/>
     </row>
-    <row r="213" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A213" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="B213" s="3"/>
-    </row>
-    <row r="214" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A214" s="6" t="s">
+    <row r="213" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A213" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="B214" s="7"/>
+      <c r="B213" s="7"/>
+    </row>
+    <row r="214" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A214" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B214" s="3"/>
     </row>
     <row r="215" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B215" s="3"/>
     </row>
     <row r="216" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A216" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B216" s="3"/>
     </row>
-    <row r="217" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A217" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="B217" s="3"/>
-    </row>
-    <row r="218" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A218" s="6" t="s">
+    <row r="217" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A217" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="B218" s="7"/>
-    </row>
-    <row r="219" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B217" s="7"/>
+    </row>
+    <row r="218" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A218" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="220" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A221" s="2" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
-        <v>311</v>
+        <v>209</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>312</v>
+        <v>209</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A223" s="2" t="s">
-        <v>209</v>
+      <c r="A223" s="5" t="s">
+        <v>313</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>209</v>
+        <v>314</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A224" s="5" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A225" s="5" t="s">
-        <v>315</v>
+      <c r="A225" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A226" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B226" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A227" s="5" t="s">
+    </row>
+    <row r="226" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A226" s="5" t="s">
         <v>317</v>
       </c>
+      <c r="B226" s="3"/>
+    </row>
+    <row r="227" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A227" s="2" t="s">
+        <v>318</v>
+      </c>
       <c r="B227" s="3"/>
     </row>
-    <row r="228" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A228" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B228" s="3"/>
     </row>
-    <row r="229" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A229" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="B229" s="3"/>
-    </row>
-    <row r="230" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>320</v>
+      </c>
+      <c r="B229" s="2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="231" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A231" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="B231" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="232" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>324</v>
+      </c>
+      <c r="B231" s="3"/>
+    </row>
+    <row r="232" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B232" s="3"/>
     </row>
-    <row r="233" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A233" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="B233" s="3"/>
-    </row>
-    <row r="234" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A234" s="6" t="s">
+    <row r="233" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A233" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="B234" s="7"/>
-    </row>
-    <row r="235" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B233" s="7"/>
+    </row>
+    <row r="234" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A234" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A235" s="2" t="s">
-        <v>143</v>
+        <v>327</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A236" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>39</v>
+        <v>329</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A237" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="B237" s="2" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="238" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A238" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B238" s="3"/>
-    </row>
-    <row r="239" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A239" s="6" t="s">
+      <c r="B237" s="3"/>
+    </row>
+    <row r="238" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A238" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="B239" s="7"/>
+      <c r="B238" s="7"/>
+    </row>
+    <row r="239" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A239" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B239" s="3"/>
     </row>
     <row r="240" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A240" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B240" s="3"/>
     </row>
     <row r="241" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A241" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B241" s="3"/>
     </row>
     <row r="242" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A242" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B242" s="3"/>
     </row>
     <row r="243" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A243" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B243" s="3"/>
     </row>
     <row r="244" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A244" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B244" s="3"/>
     </row>
     <row r="245" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A245" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B245" s="3"/>
     </row>
     <row r="246" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A246" s="2" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B246" s="3"/>
     </row>
     <row r="247" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A247" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B247" s="3"/>
     </row>
     <row r="248" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A248" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B248" s="3"/>
     </row>
     <row r="249" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A249" s="2" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B249" s="3"/>
     </row>
-    <row r="250" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A250" s="2" t="s">
-        <v>342</v>
+    <row r="250" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A250" s="5" t="s">
+        <v>343</v>
       </c>
       <c r="B250" s="3"/>
     </row>
     <row r="251" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A251" s="5" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B251" s="3"/>
     </row>
-    <row r="252" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A252" s="5" t="s">
-        <v>344</v>
+    <row r="252" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A252" s="2" t="s">
+        <v>345</v>
       </c>
       <c r="B252" s="3"/>
     </row>
     <row r="253" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A253" s="2" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B253" s="3"/>
     </row>
     <row r="254" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A254" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B254" s="3"/>
     </row>
     <row r="255" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A255" s="2" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B255" s="3"/>
     </row>
     <row r="256" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A256" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B256" s="3"/>
     </row>
     <row r="257" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A257" s="2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B257" s="3"/>
     </row>
     <row r="258" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A258" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B258" s="3"/>
     </row>
     <row r="259" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A259" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B259" s="3"/>
     </row>
     <row r="260" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A260" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B260" s="3"/>
     </row>
     <row r="261" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A261" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="B261" s="3"/>
+        <v>354</v>
+      </c>
+      <c r="B261" s="2" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="262" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A262" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>201</v>
+        <v>46</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A263" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A264" s="2" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A265" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>54</v>
+        <v>262</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A266" s="2" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="267" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A267" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A268" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="B268" s="2" t="s">
         <v>194</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A239:B239"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A204:B204"/>
-    <mergeCell ref="A214:B214"/>
-    <mergeCell ref="A218:B218"/>
-    <mergeCell ref="A234:B234"/>
+    <mergeCell ref="A238:B238"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A203:B203"/>
+    <mergeCell ref="A213:B213"/>
+    <mergeCell ref="A217:B217"/>
+    <mergeCell ref="A233:B233"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A112" r:id="rId1" display="http://lk.u.rw/" xr:uid="{B9E4BD0B-91D2-4FD4-9ABD-871EA312D809}"/>
-    <hyperlink ref="A162" r:id="rId2" display="http://lcomp.pr/" xr:uid="{403ECDDB-6691-49E3-9EF6-E88F468B06EA}"/>
-    <hyperlink ref="A164" r:id="rId3" display="http://lcomp.d.pr/" xr:uid="{C5A579A5-1E24-40B0-BF5B-A5C99625F4F7}"/>
-    <hyperlink ref="A166" r:id="rId4" display="http://acomp.pr/" xr:uid="{D7168372-AEDD-442E-9C6F-E16ABCE87316}"/>
-    <hyperlink ref="A189" r:id="rId5" display="http://u.pr/" xr:uid="{6FFAF3D3-FD95-4F54-98D3-1A67154C054E}"/>
-    <hyperlink ref="A196" r:id="rId6" display="http://l.pr/" xr:uid="{271A868E-8ED8-40B2-AAE4-23CC6B0BCAF5}"/>
-    <hyperlink ref="A199" r:id="rId7" display="http://d.pr/" xr:uid="{BC8E8F1B-AB78-46FD-A8B2-5C67E741EDD3}"/>
-    <hyperlink ref="A224" r:id="rId8" display="http://length.cv/" xr:uid="{AE5C3911-1B65-45B6-B34F-DE3F5BB36030}"/>
-    <hyperlink ref="A225" r:id="rId9" display="http://length.sd/" xr:uid="{521335C9-74F6-4BBF-B444-AF8F6173B0E5}"/>
-    <hyperlink ref="A227" r:id="rId10" display="http://wgt.mt/" xr:uid="{DC7FFAC2-4E74-41F8-A4F0-D8BB639F74C4}"/>
-    <hyperlink ref="A251" r:id="rId11" display="http://ypr.lb/" xr:uid="{AFEEA483-6DF1-4C4B-86A0-DA30CB0CC74F}"/>
-    <hyperlink ref="A252" r:id="rId12" display="http://total.lb/" xr:uid="{577BCCC4-265F-4A53-9F25-16E302A48204}"/>
+    <hyperlink ref="A111" r:id="rId1" display="http://lk.u.rw/" xr:uid="{B9E4BD0B-91D2-4FD4-9ABD-871EA312D809}"/>
+    <hyperlink ref="A161" r:id="rId2" display="http://lcomp.pr/" xr:uid="{403ECDDB-6691-49E3-9EF6-E88F468B06EA}"/>
+    <hyperlink ref="A163" r:id="rId3" display="http://lcomp.d.pr/" xr:uid="{C5A579A5-1E24-40B0-BF5B-A5C99625F4F7}"/>
+    <hyperlink ref="A165" r:id="rId4" display="http://acomp.pr/" xr:uid="{D7168372-AEDD-442E-9C6F-E16ABCE87316}"/>
+    <hyperlink ref="A188" r:id="rId5" display="http://u.pr/" xr:uid="{6FFAF3D3-FD95-4F54-98D3-1A67154C054E}"/>
+    <hyperlink ref="A195" r:id="rId6" display="http://l.pr/" xr:uid="{271A868E-8ED8-40B2-AAE4-23CC6B0BCAF5}"/>
+    <hyperlink ref="A198" r:id="rId7" display="http://d.pr/" xr:uid="{BC8E8F1B-AB78-46FD-A8B2-5C67E741EDD3}"/>
+    <hyperlink ref="A223" r:id="rId8" display="http://length.cv/" xr:uid="{AE5C3911-1B65-45B6-B34F-DE3F5BB36030}"/>
+    <hyperlink ref="A224" r:id="rId9" display="http://length.sd/" xr:uid="{521335C9-74F6-4BBF-B444-AF8F6173B0E5}"/>
+    <hyperlink ref="A226" r:id="rId10" display="http://wgt.mt/" xr:uid="{DC7FFAC2-4E74-41F8-A4F0-D8BB639F74C4}"/>
+    <hyperlink ref="A250" r:id="rId11" display="http://ypr.lb/" xr:uid="{AFEEA483-6DF1-4C4B-86A0-DA30CB0CC74F}"/>
+    <hyperlink ref="A251" r:id="rId12" display="http://total.lb/" xr:uid="{577BCCC4-265F-4A53-9F25-16E302A48204}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>

</xml_diff>

<commit_message>
Automatically identify fleet names in BAM output (#72)
* feature(find BAM fleet names)

Fix standard naming conventions sheet

* fix(convert_output):change age to numeric for converting purposes

* Update(documentation): fleet names documentation

Update create_template to reflect changes to convert_output

* Update(convert_output): fleet names not kept in D.release/Dosed.release

* Deprecate fleet_names parameter in create_template

* Update documentation for PR

* Fix(create_template): species naming in converted output within create_template

* fix(convert_output): add nsim factor

Nsim factor in BAM for eq.series and pr.series - might need further adjustment for naming (unsure if nsim)

* fix(convert_output test): reflect the new factor added to the output file

* fix(convert_output): aging error matrix for BAM incorrectly transformed

Reflect the changes and addition of another factor into the test
</commit_message>
<xml_diff>
--- a/inst/resources/bam_var_names.xlsx
+++ b/inst/resources/bam_var_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samantha.schiano\Documents\GitHub-Repos\asar\inst\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B415980-1889-4528-B410-4050CA4FABD5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C32A076-F542-4B00-B7CD-2899A4A7399D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10404" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="375">
   <si>
     <t>label</t>
   </si>
@@ -1488,10 +1488,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B268"/>
+  <dimension ref="A1:B267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="B247" sqref="B247"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1548,79 +1548,81 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>11</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>365</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>23</v>
@@ -1628,7 +1630,7 @@
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>23</v>
@@ -1636,7 +1638,7 @@
     </row>
     <row r="19" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>23</v>
@@ -1644,7 +1646,7 @@
     </row>
     <row r="20" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>23</v>
@@ -1652,43 +1654,43 @@
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B23" s="3"/>
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B24" s="3"/>
     </row>
     <row r="25" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>366</v>
@@ -1696,7 +1698,7 @@
     </row>
     <row r="27" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>366</v>
@@ -1704,7 +1706,7 @@
     </row>
     <row r="28" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>366</v>
@@ -1712,1720 +1714,1712 @@
     </row>
     <row r="29" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>56</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="B39" s="3"/>
     </row>
     <row r="40" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B41" s="3"/>
     </row>
     <row r="42" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B42" s="3"/>
-    </row>
-    <row r="43" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>123</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>54</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="B44" s="3"/>
     </row>
     <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B45" s="3"/>
     </row>
     <row r="46" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B46" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="47" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>370</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>88</v>
+        <v>371</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>23</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="B68" s="3"/>
     </row>
     <row r="69" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B69" s="3"/>
     </row>
     <row r="70" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B70" s="3"/>
-    </row>
-    <row r="71" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>113</v>
+        <v>13</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>114</v>
+        <v>13</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="B78" s="3"/>
     </row>
     <row r="79" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B79" s="3"/>
+        <v>116</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="80" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>123</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="B83" s="3"/>
     </row>
     <row r="84" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B84" s="3"/>
     </row>
     <row r="85" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B85" s="3"/>
     </row>
-    <row r="86" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B86" s="3"/>
-    </row>
-    <row r="87" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="6" t="s">
+    <row r="86" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="B87" s="7"/>
+      <c r="B86" s="7"/>
+    </row>
+    <row r="87" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B87" s="3"/>
     </row>
     <row r="88" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B88" s="3"/>
     </row>
-    <row r="89" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B89" s="3"/>
-    </row>
-    <row r="90" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>9</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="B96" s="3"/>
     </row>
     <row r="97" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B97" s="3"/>
     </row>
     <row r="98" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B98" s="3"/>
     </row>
     <row r="99" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B99" s="3"/>
     </row>
     <row r="100" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B100" s="3"/>
-    </row>
-    <row r="101" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>372</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="B101" s="3"/>
     </row>
     <row r="102" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B102" s="3"/>
     </row>
     <row r="103" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B103" s="3"/>
     </row>
     <row r="104" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B104" s="3"/>
     </row>
     <row r="105" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B105" s="3"/>
     </row>
     <row r="106" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B106" s="3"/>
     </row>
     <row r="107" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B107" s="3"/>
     </row>
     <row r="108" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B108" s="3"/>
     </row>
     <row r="109" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B109" s="3"/>
     </row>
     <row r="110" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B110" s="3"/>
     </row>
-    <row r="111" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="2" t="s">
-        <v>158</v>
+    <row r="111" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="5" t="s">
+        <v>159</v>
       </c>
       <c r="B111" s="3"/>
     </row>
-    <row r="112" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="5" t="s">
-        <v>159</v>
+    <row r="112" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="2" t="s">
+        <v>160</v>
       </c>
       <c r="B112" s="3"/>
     </row>
     <row r="113" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B113" s="3"/>
     </row>
     <row r="114" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B114" s="3"/>
     </row>
     <row r="115" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B115" s="3"/>
-    </row>
-    <row r="116" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>264</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="B117" s="3"/>
     </row>
     <row r="118" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B118" s="3"/>
     </row>
     <row r="119" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B119" s="3"/>
     </row>
     <row r="120" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B120" s="3"/>
     </row>
     <row r="121" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B121" s="3"/>
     </row>
     <row r="122" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B122" s="3"/>
     </row>
     <row r="123" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B123" s="3"/>
     </row>
     <row r="124" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B124" s="3"/>
     </row>
     <row r="125" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B125" s="3"/>
     </row>
     <row r="126" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B126" s="3"/>
-    </row>
-    <row r="127" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>187</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="B133" s="3"/>
     </row>
     <row r="134" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B134" s="3"/>
     </row>
     <row r="135" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B135" s="3"/>
-    </row>
-    <row r="136" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>191</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="B136" s="3"/>
     </row>
     <row r="137" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B137" s="3"/>
+        <v>193</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="138" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>198</v>
+        <v>42</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="B146" s="2" t="s">
-        <v>209</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="B146" s="3"/>
     </row>
     <row r="147" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B147" s="3"/>
     </row>
     <row r="148" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B148" s="3"/>
     </row>
     <row r="149" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B149" s="3"/>
+        <v>213</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="150" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="B150" s="2" t="s">
-        <v>214</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="B150" s="3"/>
     </row>
     <row r="151" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B151" s="3"/>
     </row>
     <row r="152" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B152" s="3"/>
     </row>
     <row r="153" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B153" s="3"/>
     </row>
     <row r="154" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B154" s="3"/>
     </row>
     <row r="155" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B155" s="3"/>
     </row>
-    <row r="156" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B156" s="3"/>
     </row>
     <row r="157" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B157" s="3"/>
     </row>
     <row r="158" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B158" s="3"/>
     </row>
     <row r="159" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B159" s="3"/>
     </row>
     <row r="160" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B160" s="3"/>
-    </row>
-    <row r="161" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="2" t="s">
         <v>225</v>
       </c>
+      <c r="B160" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A161" s="5" t="s">
+        <v>227</v>
+      </c>
       <c r="B161" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="5" t="s">
-        <v>227</v>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A162" s="2" t="s">
+        <v>229</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A163" s="5" t="s">
+        <v>231</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="5" t="s">
-        <v>231</v>
+        <v>232</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A164" s="2" t="s">
+        <v>233</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A165" s="5" t="s">
+        <v>235</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A166" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="B166" s="2" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A166" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B166" s="3"/>
+    </row>
+    <row r="167" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B167" s="3"/>
     </row>
-    <row r="168" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B168" s="3"/>
     </row>
     <row r="169" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="B169" s="3"/>
+        <v>240</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="170" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>201</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="B172" s="3"/>
     </row>
     <row r="173" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="B173" s="3"/>
-    </row>
-    <row r="174" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>244</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>374</v>
+        <v>194</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>194</v>
+        <v>54</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>361</v>
+        <v>249</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="B182" s="2" t="s">
-        <v>257</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="B182" s="3"/>
     </row>
     <row r="183" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="B183" s="3"/>
-    </row>
-    <row r="184" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A188" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A188" s="5" t="s">
+        <v>269</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A189" s="5" t="s">
-        <v>269</v>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A189" s="2" t="s">
+        <v>271</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="B191" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>274</v>
+      </c>
+      <c r="B191" s="3"/>
     </row>
     <row r="192" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B192" s="3"/>
     </row>
     <row r="193" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B193" s="3"/>
     </row>
     <row r="194" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="B194" s="3"/>
-    </row>
-    <row r="195" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A195" s="2" t="s">
         <v>277</v>
       </c>
+      <c r="B194" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A195" s="5" t="s">
+        <v>279</v>
+      </c>
       <c r="B195" s="2" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="5" t="s">
-        <v>279</v>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A196" s="2" t="s">
+        <v>281</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A198" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A198" s="5" t="s">
+        <v>285</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A199" s="5" t="s">
-        <v>285</v>
+        <v>286</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A199" s="2" t="s">
+        <v>287</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="B200" s="2" t="s">
-        <v>288</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="B200" s="3"/>
     </row>
     <row r="201" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B201" s="3"/>
     </row>
-    <row r="202" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A202" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B202" s="3"/>
     </row>
-    <row r="203" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A203" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="B203" s="3"/>
-    </row>
-    <row r="204" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A204" s="6" t="s">
+    <row r="203" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A203" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B204" s="7"/>
+      <c r="B203" s="7"/>
+    </row>
+    <row r="204" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A204" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B204" s="3"/>
     </row>
     <row r="205" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B205" s="3"/>
     </row>
-    <row r="206" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B206" s="3"/>
     </row>
     <row r="207" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A207" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B207" s="3"/>
     </row>
     <row r="208" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B208" s="3"/>
     </row>
     <row r="209" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A209" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B209" s="3"/>
     </row>
-    <row r="210" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B210" s="3"/>
     </row>
     <row r="211" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B211" s="3"/>
     </row>
     <row r="212" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B212" s="3"/>
     </row>
-    <row r="213" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A213" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="B213" s="3"/>
-    </row>
-    <row r="214" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A214" s="6" t="s">
+    <row r="213" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A213" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="B214" s="7"/>
+      <c r="B213" s="7"/>
+    </row>
+    <row r="214" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A214" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B214" s="3"/>
     </row>
     <row r="215" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B215" s="3"/>
     </row>
     <row r="216" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A216" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B216" s="3"/>
     </row>
-    <row r="217" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A217" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="B217" s="3"/>
-    </row>
-    <row r="218" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A218" s="6" t="s">
+    <row r="217" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A217" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="B218" s="7"/>
-    </row>
-    <row r="219" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B217" s="7"/>
+    </row>
+    <row r="218" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A218" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="220" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A221" s="2" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
-        <v>311</v>
+        <v>209</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>312</v>
+        <v>209</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A223" s="2" t="s">
-        <v>209</v>
+      <c r="A223" s="5" t="s">
+        <v>313</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>209</v>
+        <v>314</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A224" s="5" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A225" s="5" t="s">
-        <v>315</v>
+      <c r="A225" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A226" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B226" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A227" s="5" t="s">
+    </row>
+    <row r="226" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A226" s="5" t="s">
         <v>317</v>
       </c>
+      <c r="B226" s="3"/>
+    </row>
+    <row r="227" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A227" s="2" t="s">
+        <v>318</v>
+      </c>
       <c r="B227" s="3"/>
     </row>
-    <row r="228" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A228" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B228" s="3"/>
     </row>
-    <row r="229" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A229" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="B229" s="3"/>
-    </row>
-    <row r="230" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>320</v>
+      </c>
+      <c r="B229" s="2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="231" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A231" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="B231" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="232" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+        <v>324</v>
+      </c>
+      <c r="B231" s="3"/>
+    </row>
+    <row r="232" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B232" s="3"/>
     </row>
-    <row r="233" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A233" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="B233" s="3"/>
-    </row>
-    <row r="234" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A234" s="6" t="s">
+    <row r="233" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A233" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="B234" s="7"/>
-    </row>
-    <row r="235" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B233" s="7"/>
+    </row>
+    <row r="234" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A234" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A235" s="2" t="s">
-        <v>143</v>
+        <v>327</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A236" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>39</v>
+        <v>329</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A237" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="B237" s="2" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="238" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A238" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B238" s="3"/>
-    </row>
-    <row r="239" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A239" s="6" t="s">
+      <c r="B237" s="3"/>
+    </row>
+    <row r="238" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A238" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="B239" s="7"/>
+      <c r="B238" s="7"/>
+    </row>
+    <row r="239" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A239" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B239" s="3"/>
     </row>
     <row r="240" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A240" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B240" s="3"/>
     </row>
     <row r="241" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A241" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B241" s="3"/>
     </row>
     <row r="242" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A242" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B242" s="3"/>
     </row>
     <row r="243" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A243" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B243" s="3"/>
     </row>
     <row r="244" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A244" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B244" s="3"/>
     </row>
     <row r="245" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A245" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B245" s="3"/>
     </row>
     <row r="246" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A246" s="2" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B246" s="3"/>
     </row>
     <row r="247" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A247" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B247" s="3"/>
     </row>
     <row r="248" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A248" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B248" s="3"/>
     </row>
     <row r="249" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A249" s="2" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B249" s="3"/>
     </row>
-    <row r="250" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A250" s="2" t="s">
-        <v>342</v>
+    <row r="250" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A250" s="5" t="s">
+        <v>343</v>
       </c>
       <c r="B250" s="3"/>
     </row>
     <row r="251" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A251" s="5" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B251" s="3"/>
     </row>
-    <row r="252" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A252" s="5" t="s">
-        <v>344</v>
+    <row r="252" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A252" s="2" t="s">
+        <v>345</v>
       </c>
       <c r="B252" s="3"/>
     </row>
     <row r="253" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A253" s="2" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B253" s="3"/>
     </row>
     <row r="254" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A254" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B254" s="3"/>
     </row>
     <row r="255" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A255" s="2" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B255" s="3"/>
     </row>
     <row r="256" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A256" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B256" s="3"/>
     </row>
     <row r="257" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A257" s="2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B257" s="3"/>
     </row>
     <row r="258" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A258" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B258" s="3"/>
     </row>
     <row r="259" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A259" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B259" s="3"/>
     </row>
     <row r="260" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A260" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B260" s="3"/>
     </row>
     <row r="261" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A261" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="B261" s="3"/>
+        <v>354</v>
+      </c>
+      <c r="B261" s="2" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="262" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A262" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>201</v>
+        <v>46</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A263" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A264" s="2" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A265" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>54</v>
+        <v>262</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A266" s="2" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="267" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A267" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A268" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="B268" s="2" t="s">
         <v>194</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A239:B239"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A204:B204"/>
-    <mergeCell ref="A214:B214"/>
-    <mergeCell ref="A218:B218"/>
-    <mergeCell ref="A234:B234"/>
+    <mergeCell ref="A238:B238"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A203:B203"/>
+    <mergeCell ref="A213:B213"/>
+    <mergeCell ref="A217:B217"/>
+    <mergeCell ref="A233:B233"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A112" r:id="rId1" display="http://lk.u.rw/" xr:uid="{B9E4BD0B-91D2-4FD4-9ABD-871EA312D809}"/>
-    <hyperlink ref="A162" r:id="rId2" display="http://lcomp.pr/" xr:uid="{403ECDDB-6691-49E3-9EF6-E88F468B06EA}"/>
-    <hyperlink ref="A164" r:id="rId3" display="http://lcomp.d.pr/" xr:uid="{C5A579A5-1E24-40B0-BF5B-A5C99625F4F7}"/>
-    <hyperlink ref="A166" r:id="rId4" display="http://acomp.pr/" xr:uid="{D7168372-AEDD-442E-9C6F-E16ABCE87316}"/>
-    <hyperlink ref="A189" r:id="rId5" display="http://u.pr/" xr:uid="{6FFAF3D3-FD95-4F54-98D3-1A67154C054E}"/>
-    <hyperlink ref="A196" r:id="rId6" display="http://l.pr/" xr:uid="{271A868E-8ED8-40B2-AAE4-23CC6B0BCAF5}"/>
-    <hyperlink ref="A199" r:id="rId7" display="http://d.pr/" xr:uid="{BC8E8F1B-AB78-46FD-A8B2-5C67E741EDD3}"/>
-    <hyperlink ref="A224" r:id="rId8" display="http://length.cv/" xr:uid="{AE5C3911-1B65-45B6-B34F-DE3F5BB36030}"/>
-    <hyperlink ref="A225" r:id="rId9" display="http://length.sd/" xr:uid="{521335C9-74F6-4BBF-B444-AF8F6173B0E5}"/>
-    <hyperlink ref="A227" r:id="rId10" display="http://wgt.mt/" xr:uid="{DC7FFAC2-4E74-41F8-A4F0-D8BB639F74C4}"/>
-    <hyperlink ref="A251" r:id="rId11" display="http://ypr.lb/" xr:uid="{AFEEA483-6DF1-4C4B-86A0-DA30CB0CC74F}"/>
-    <hyperlink ref="A252" r:id="rId12" display="http://total.lb/" xr:uid="{577BCCC4-265F-4A53-9F25-16E302A48204}"/>
+    <hyperlink ref="A111" r:id="rId1" display="http://lk.u.rw/" xr:uid="{B9E4BD0B-91D2-4FD4-9ABD-871EA312D809}"/>
+    <hyperlink ref="A161" r:id="rId2" display="http://lcomp.pr/" xr:uid="{403ECDDB-6691-49E3-9EF6-E88F468B06EA}"/>
+    <hyperlink ref="A163" r:id="rId3" display="http://lcomp.d.pr/" xr:uid="{C5A579A5-1E24-40B0-BF5B-A5C99625F4F7}"/>
+    <hyperlink ref="A165" r:id="rId4" display="http://acomp.pr/" xr:uid="{D7168372-AEDD-442E-9C6F-E16ABCE87316}"/>
+    <hyperlink ref="A188" r:id="rId5" display="http://u.pr/" xr:uid="{6FFAF3D3-FD95-4F54-98D3-1A67154C054E}"/>
+    <hyperlink ref="A195" r:id="rId6" display="http://l.pr/" xr:uid="{271A868E-8ED8-40B2-AAE4-23CC6B0BCAF5}"/>
+    <hyperlink ref="A198" r:id="rId7" display="http://d.pr/" xr:uid="{BC8E8F1B-AB78-46FD-A8B2-5C67E741EDD3}"/>
+    <hyperlink ref="A223" r:id="rId8" display="http://length.cv/" xr:uid="{AE5C3911-1B65-45B6-B34F-DE3F5BB36030}"/>
+    <hyperlink ref="A224" r:id="rId9" display="http://length.sd/" xr:uid="{521335C9-74F6-4BBF-B444-AF8F6173B0E5}"/>
+    <hyperlink ref="A226" r:id="rId10" display="http://wgt.mt/" xr:uid="{DC7FFAC2-4E74-41F8-A4F0-D8BB639F74C4}"/>
+    <hyperlink ref="A250" r:id="rId11" display="http://ypr.lb/" xr:uid="{AFEEA483-6DF1-4C4B-86A0-DA30CB0CC74F}"/>
+    <hyperlink ref="A251" r:id="rId12" display="http://total.lb/" xr:uid="{577BCCC4-265F-4A53-9F25-16E302A48204}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>

</xml_diff>

<commit_message>
update(bam_var_names): spelling on recruitment deviations
</commit_message>
<xml_diff>
--- a/inst/resources/bam_var_names.xlsx
+++ b/inst/resources/bam_var_names.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samantha.schiano\Documents\GitHub-Repos\asar\inst\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samantha.schiano\Documents\GitHub\asar\inst\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C32A076-F542-4B00-B7CD-2899A4A7399D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10404" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10400"/>
   </bookViews>
   <sheets>
     <sheet name="bam_var_names" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="374">
   <si>
     <t>label</t>
   </si>
@@ -575,9 +574,6 @@
   </si>
   <si>
     <t>log.rec.dev</t>
-  </si>
-  <si>
-    <t>log_recruitment_devitations</t>
   </si>
   <si>
     <t>log.F.dev</t>
@@ -1150,7 +1146,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1484,20 +1480,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:B267"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="B176" sqref="B176"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.77734375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="28.6328125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1565,7 +1561,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1573,7 +1569,7 @@
         <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1581,7 +1577,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1589,7 +1585,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1685,7 +1681,7 @@
         <v>34</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1693,7 +1689,7 @@
         <v>35</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1701,7 +1697,7 @@
         <v>36</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1709,7 +1705,7 @@
         <v>37</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1717,7 +1713,7 @@
         <v>38</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1725,7 +1721,7 @@
         <v>40</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1752,7 +1748,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>47</v>
       </c>
@@ -1760,7 +1756,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>49</v>
       </c>
@@ -1859,7 +1855,7 @@
         <v>68</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1891,7 +1887,7 @@
         <v>74</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1934,7 +1930,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>85</v>
       </c>
@@ -1955,7 +1951,7 @@
         <v>89</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -2066,7 +2062,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>111</v>
       </c>
@@ -2074,7 +2070,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>113</v>
       </c>
@@ -2146,7 +2142,7 @@
       </c>
       <c r="B85" s="3"/>
     </row>
-    <row r="86" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A86" s="6" t="s">
         <v>127</v>
       </c>
@@ -2196,7 +2192,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>138</v>
       </c>
@@ -2249,7 +2245,7 @@
         <v>148</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -2312,7 +2308,7 @@
       </c>
       <c r="B110" s="3"/>
     </row>
-    <row r="111" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>159</v>
       </c>
@@ -2341,7 +2337,7 @@
         <v>163</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -2349,7 +2345,7 @@
         <v>164</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -2414,7 +2410,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>176</v>
       </c>
@@ -2422,7 +2418,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>178</v>
       </c>
@@ -2430,7 +2426,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:2" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>180</v>
       </c>
@@ -2438,7 +2434,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:2" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>182</v>
       </c>
@@ -2451,70 +2447,70 @@
         <v>184</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>185</v>
+        <v>360</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B132" s="2" t="s">
         <v>186</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B133" s="3"/>
     </row>
     <row r="134" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B134" s="3"/>
     </row>
     <row r="135" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B135" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B136" s="3"/>
     </row>
     <row r="137" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B137" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B138" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B139" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>42</v>
@@ -2522,199 +2518,199 @@
     </row>
     <row r="141" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B141" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B142" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B143" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="B143" s="2" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B144" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B145" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="B145" s="2" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B146" s="3"/>
     </row>
     <row r="147" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B147" s="3"/>
     </row>
     <row r="148" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B148" s="3"/>
     </row>
     <row r="149" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B149" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B150" s="3"/>
     </row>
     <row r="151" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B151" s="3"/>
     </row>
     <row r="152" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B152" s="3"/>
     </row>
     <row r="153" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B153" s="3"/>
     </row>
     <row r="154" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B154" s="3"/>
     </row>
     <row r="155" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B155" s="3"/>
     </row>
     <row r="156" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B156" s="3"/>
     </row>
     <row r="157" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B157" s="3"/>
     </row>
     <row r="158" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B158" s="3"/>
     </row>
     <row r="159" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B159" s="3"/>
     </row>
     <row r="160" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B160" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="B160" s="2" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="B161" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="B161" s="2" t="s">
+    </row>
+    <row r="162" spans="1:2" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A162" s="2" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="162" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="2" t="s">
+      <c r="B162" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B162" s="2" t="s">
+    </row>
+    <row r="163" spans="1:2" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A163" s="5" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="163" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="5" t="s">
+      <c r="B163" s="2" t="s">
         <v>231</v>
-      </c>
-      <c r="B163" s="2" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B164" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="B164" s="2" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B165" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="B165" s="2" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B166" s="3"/>
     </row>
     <row r="167" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B167" s="3"/>
     </row>
     <row r="168" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B168" s="3"/>
     </row>
     <row r="169" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B169" s="2" t="s">
         <v>82</v>
@@ -2722,45 +2718,45 @@
     </row>
     <row r="170" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B172" s="3"/>
     </row>
     <row r="173" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B175" s="2" t="s">
         <v>54</v>
@@ -2768,117 +2764,117 @@
     </row>
     <row r="176" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B177" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B178" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B179" s="2" t="s">
         <v>252</v>
-      </c>
-      <c r="B179" s="2" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B180" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="B180" s="2" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B181" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="B181" s="2" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B182" s="3"/>
     </row>
     <row r="183" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B183" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="B183" s="2" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B184" s="2" t="s">
         <v>261</v>
-      </c>
-      <c r="B184" s="2" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B185" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="B185" s="2" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B186" s="2" t="s">
         <v>265</v>
-      </c>
-      <c r="B186" s="2" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B187" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="B187" s="2" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="B188" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="B188" s="2" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B189" s="2" t="s">
         <v>271</v>
-      </c>
-      <c r="B189" s="2" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B190" s="2" t="s">
         <v>31</v>
@@ -2886,291 +2882,291 @@
     </row>
     <row r="191" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B191" s="3"/>
     </row>
     <row r="192" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B192" s="3"/>
     </row>
     <row r="193" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B193" s="3"/>
     </row>
     <row r="194" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B194" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="B194" s="2" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="B195" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="B195" s="2" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B196" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="B196" s="2" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B197" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="B197" s="2" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B198" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="B198" s="2" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B199" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="B199" s="2" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B200" s="3"/>
     </row>
     <row r="201" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B201" s="3"/>
     </row>
     <row r="202" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A202" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B202" s="3"/>
+    </row>
+    <row r="203" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A203" s="6" t="s">
         <v>291</v>
-      </c>
-      <c r="B202" s="3"/>
-    </row>
-    <row r="203" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A203" s="6" t="s">
-        <v>292</v>
       </c>
       <c r="B203" s="7"/>
     </row>
     <row r="204" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B204" s="3"/>
     </row>
     <row r="205" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B205" s="3"/>
     </row>
     <row r="206" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B206" s="3"/>
     </row>
     <row r="207" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A207" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B207" s="3"/>
     </row>
     <row r="208" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B208" s="3"/>
     </row>
     <row r="209" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A209" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B209" s="3"/>
     </row>
     <row r="210" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B210" s="3"/>
     </row>
     <row r="211" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B211" s="3"/>
     </row>
     <row r="212" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B212" s="3"/>
+    </row>
+    <row r="213" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A213" s="6" t="s">
         <v>301</v>
-      </c>
-      <c r="B212" s="3"/>
-    </row>
-    <row r="213" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A213" s="6" t="s">
-        <v>302</v>
       </c>
       <c r="B213" s="7"/>
     </row>
     <row r="214" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B214" s="3"/>
     </row>
     <row r="215" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B215" s="3"/>
     </row>
     <row r="216" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A216" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B216" s="3"/>
+    </row>
+    <row r="217" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A217" s="6" t="s">
         <v>305</v>
-      </c>
-      <c r="B216" s="3"/>
-    </row>
-    <row r="217" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A217" s="6" t="s">
-        <v>306</v>
       </c>
       <c r="B217" s="7"/>
     </row>
     <row r="218" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A218" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B220" s="2" t="s">
         <v>309</v>
-      </c>
-      <c r="B220" s="2" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A221" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B221" s="2" t="s">
         <v>311</v>
-      </c>
-      <c r="B221" s="2" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A223" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="B223" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="B223" s="2" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A224" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="B224" s="2" t="s">
         <v>315</v>
-      </c>
-      <c r="B224" s="2" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A226" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B226" s="3"/>
     </row>
     <row r="227" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A227" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B227" s="3"/>
     </row>
     <row r="228" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A228" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B228" s="3"/>
     </row>
     <row r="229" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A229" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B229" s="2" t="s">
         <v>320</v>
-      </c>
-      <c r="B229" s="2" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B230" s="2" t="s">
         <v>322</v>
-      </c>
-      <c r="B230" s="2" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A231" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B231" s="3"/>
     </row>
     <row r="232" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B232" s="3"/>
+    </row>
+    <row r="233" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A233" s="6" t="s">
         <v>325</v>
-      </c>
-      <c r="B232" s="3"/>
-    </row>
-    <row r="233" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A233" s="6" t="s">
-        <v>326</v>
       </c>
       <c r="B233" s="7"/>
     </row>
@@ -3184,7 +3180,7 @@
     </row>
     <row r="235" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A235" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B235" s="2" t="s">
         <v>39</v>
@@ -3192,167 +3188,167 @@
     </row>
     <row r="236" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A236" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B236" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="B236" s="2" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A237" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B237" s="3"/>
+    </row>
+    <row r="238" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A238" s="6" t="s">
         <v>330</v>
-      </c>
-      <c r="B237" s="3"/>
-    </row>
-    <row r="238" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A238" s="6" t="s">
-        <v>331</v>
       </c>
       <c r="B238" s="7"/>
     </row>
     <row r="239" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A239" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B239" s="3"/>
     </row>
     <row r="240" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A240" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B240" s="3"/>
     </row>
     <row r="241" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A241" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B241" s="3"/>
     </row>
     <row r="242" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A242" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B242" s="3"/>
     </row>
     <row r="243" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A243" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B243" s="3"/>
     </row>
     <row r="244" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A244" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B244" s="3"/>
     </row>
     <row r="245" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A245" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B245" s="3"/>
     </row>
     <row r="246" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A246" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B246" s="3"/>
     </row>
     <row r="247" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A247" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B247" s="3"/>
     </row>
     <row r="248" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A248" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B248" s="3"/>
     </row>
     <row r="249" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A249" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B249" s="3"/>
+    </row>
+    <row r="250" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A250" s="5" t="s">
         <v>342</v>
       </c>
-      <c r="B249" s="3"/>
-    </row>
-    <row r="250" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A250" s="5" t="s">
+      <c r="B250" s="3"/>
+    </row>
+    <row r="251" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A251" s="5" t="s">
         <v>343</v>
-      </c>
-      <c r="B250" s="3"/>
-    </row>
-    <row r="251" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A251" s="5" t="s">
-        <v>344</v>
       </c>
       <c r="B251" s="3"/>
     </row>
     <row r="252" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A252" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B252" s="3"/>
     </row>
     <row r="253" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A253" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B253" s="3"/>
     </row>
     <row r="254" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A254" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B254" s="3"/>
     </row>
     <row r="255" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A255" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B255" s="3"/>
     </row>
     <row r="256" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A256" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B256" s="3"/>
     </row>
     <row r="257" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A257" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B257" s="3"/>
     </row>
     <row r="258" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A258" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B258" s="3"/>
     </row>
     <row r="259" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A259" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B259" s="3"/>
     </row>
     <row r="260" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A260" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B260" s="3"/>
     </row>
     <row r="261" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A261" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A262" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B262" s="2" t="s">
         <v>46</v>
@@ -3360,7 +3356,7 @@
     </row>
     <row r="263" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A263" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B263" s="2" t="s">
         <v>42</v>
@@ -3368,7 +3364,7 @@
     </row>
     <row r="264" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A264" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B264" s="2" t="s">
         <v>54</v>
@@ -3376,26 +3372,26 @@
     </row>
     <row r="265" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A265" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A266" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A267" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -3408,18 +3404,18 @@
     <mergeCell ref="A233:B233"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A111" r:id="rId1" display="http://lk.u.rw/" xr:uid="{B9E4BD0B-91D2-4FD4-9ABD-871EA312D809}"/>
-    <hyperlink ref="A161" r:id="rId2" display="http://lcomp.pr/" xr:uid="{403ECDDB-6691-49E3-9EF6-E88F468B06EA}"/>
-    <hyperlink ref="A163" r:id="rId3" display="http://lcomp.d.pr/" xr:uid="{C5A579A5-1E24-40B0-BF5B-A5C99625F4F7}"/>
-    <hyperlink ref="A165" r:id="rId4" display="http://acomp.pr/" xr:uid="{D7168372-AEDD-442E-9C6F-E16ABCE87316}"/>
-    <hyperlink ref="A188" r:id="rId5" display="http://u.pr/" xr:uid="{6FFAF3D3-FD95-4F54-98D3-1A67154C054E}"/>
-    <hyperlink ref="A195" r:id="rId6" display="http://l.pr/" xr:uid="{271A868E-8ED8-40B2-AAE4-23CC6B0BCAF5}"/>
-    <hyperlink ref="A198" r:id="rId7" display="http://d.pr/" xr:uid="{BC8E8F1B-AB78-46FD-A8B2-5C67E741EDD3}"/>
-    <hyperlink ref="A223" r:id="rId8" display="http://length.cv/" xr:uid="{AE5C3911-1B65-45B6-B34F-DE3F5BB36030}"/>
-    <hyperlink ref="A224" r:id="rId9" display="http://length.sd/" xr:uid="{521335C9-74F6-4BBF-B444-AF8F6173B0E5}"/>
-    <hyperlink ref="A226" r:id="rId10" display="http://wgt.mt/" xr:uid="{DC7FFAC2-4E74-41F8-A4F0-D8BB639F74C4}"/>
-    <hyperlink ref="A250" r:id="rId11" display="http://ypr.lb/" xr:uid="{AFEEA483-6DF1-4C4B-86A0-DA30CB0CC74F}"/>
-    <hyperlink ref="A251" r:id="rId12" display="http://total.lb/" xr:uid="{577BCCC4-265F-4A53-9F25-16E302A48204}"/>
+    <hyperlink ref="A111" r:id="rId1" display="http://lk.u.rw/"/>
+    <hyperlink ref="A161" r:id="rId2" display="http://lcomp.pr/"/>
+    <hyperlink ref="A163" r:id="rId3" display="http://lcomp.d.pr/"/>
+    <hyperlink ref="A165" r:id="rId4" display="http://acomp.pr/"/>
+    <hyperlink ref="A188" r:id="rId5" display="http://u.pr/"/>
+    <hyperlink ref="A195" r:id="rId6" display="http://l.pr/"/>
+    <hyperlink ref="A198" r:id="rId7" display="http://d.pr/"/>
+    <hyperlink ref="A223" r:id="rId8" display="http://length.cv/"/>
+    <hyperlink ref="A224" r:id="rId9" display="http://length.sd/"/>
+    <hyperlink ref="A226" r:id="rId10" display="http://wgt.mt/"/>
+    <hyperlink ref="A250" r:id="rId11" display="http://ypr.lb/"/>
+    <hyperlink ref="A251" r:id="rId12" display="http://total.lb/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>

</xml_diff>

<commit_message>
Bug fix to recent release (#80)
* fix(species naming): replace all spaces with underscore when str_replace is used

* fix(create_title): removing duplicate wording in title

Issue was that in the NWFSC , the region "U.S. West Coast" did not make sense in the context of the created title

* fix(create_tables/figures_doc): reflect changes to dat where its read in in preamble in skeleton rather than each plot

* update(bam_var_names): spelling on recruitment deviations

* update(ss3_var_names): make adjustments to std naming conversion
</commit_message>
<xml_diff>
--- a/inst/resources/bam_var_names.xlsx
+++ b/inst/resources/bam_var_names.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samantha.schiano\Documents\GitHub-Repos\asar\inst\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samantha.schiano\Documents\GitHub\asar\inst\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C32A076-F542-4B00-B7CD-2899A4A7399D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10404" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10400"/>
   </bookViews>
   <sheets>
     <sheet name="bam_var_names" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="374">
   <si>
     <t>label</t>
   </si>
@@ -575,9 +574,6 @@
   </si>
   <si>
     <t>log.rec.dev</t>
-  </si>
-  <si>
-    <t>log_recruitment_devitations</t>
   </si>
   <si>
     <t>log.F.dev</t>
@@ -1150,7 +1146,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1484,20 +1480,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:B267"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="B176" sqref="B176"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.77734375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="28.6328125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1565,7 +1561,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1573,7 +1569,7 @@
         <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1581,7 +1577,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1589,7 +1585,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1685,7 +1681,7 @@
         <v>34</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1693,7 +1689,7 @@
         <v>35</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1701,7 +1697,7 @@
         <v>36</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1709,7 +1705,7 @@
         <v>37</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1717,7 +1713,7 @@
         <v>38</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1725,7 +1721,7 @@
         <v>40</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1752,7 +1748,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>47</v>
       </c>
@@ -1760,7 +1756,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>49</v>
       </c>
@@ -1859,7 +1855,7 @@
         <v>68</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1891,7 +1887,7 @@
         <v>74</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1934,7 +1930,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>85</v>
       </c>
@@ -1955,7 +1951,7 @@
         <v>89</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -2066,7 +2062,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>111</v>
       </c>
@@ -2074,7 +2070,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>113</v>
       </c>
@@ -2146,7 +2142,7 @@
       </c>
       <c r="B85" s="3"/>
     </row>
-    <row r="86" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A86" s="6" t="s">
         <v>127</v>
       </c>
@@ -2196,7 +2192,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>138</v>
       </c>
@@ -2249,7 +2245,7 @@
         <v>148</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -2312,7 +2308,7 @@
       </c>
       <c r="B110" s="3"/>
     </row>
-    <row r="111" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>159</v>
       </c>
@@ -2341,7 +2337,7 @@
         <v>163</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -2349,7 +2345,7 @@
         <v>164</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -2414,7 +2410,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>176</v>
       </c>
@@ -2422,7 +2418,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>178</v>
       </c>
@@ -2430,7 +2426,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:2" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>180</v>
       </c>
@@ -2438,7 +2434,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:2" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>182</v>
       </c>
@@ -2451,70 +2447,70 @@
         <v>184</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>185</v>
+        <v>360</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B132" s="2" t="s">
         <v>186</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B133" s="3"/>
     </row>
     <row r="134" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B134" s="3"/>
     </row>
     <row r="135" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B135" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B136" s="3"/>
     </row>
     <row r="137" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B137" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B138" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B139" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>42</v>
@@ -2522,199 +2518,199 @@
     </row>
     <row r="141" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B141" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B142" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B143" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="B143" s="2" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B144" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B145" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="B145" s="2" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B146" s="3"/>
     </row>
     <row r="147" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B147" s="3"/>
     </row>
     <row r="148" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B148" s="3"/>
     </row>
     <row r="149" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B149" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B150" s="3"/>
     </row>
     <row r="151" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B151" s="3"/>
     </row>
     <row r="152" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B152" s="3"/>
     </row>
     <row r="153" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B153" s="3"/>
     </row>
     <row r="154" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B154" s="3"/>
     </row>
     <row r="155" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B155" s="3"/>
     </row>
     <row r="156" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B156" s="3"/>
     </row>
     <row r="157" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B157" s="3"/>
     </row>
     <row r="158" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B158" s="3"/>
     </row>
     <row r="159" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B159" s="3"/>
     </row>
     <row r="160" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B160" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="B160" s="2" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="B161" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="B161" s="2" t="s">
+    </row>
+    <row r="162" spans="1:2" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A162" s="2" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="162" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="2" t="s">
+      <c r="B162" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B162" s="2" t="s">
+    </row>
+    <row r="163" spans="1:2" ht="29.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A163" s="5" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="163" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="5" t="s">
+      <c r="B163" s="2" t="s">
         <v>231</v>
-      </c>
-      <c r="B163" s="2" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B164" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="B164" s="2" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B165" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="B165" s="2" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B166" s="3"/>
     </row>
     <row r="167" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B167" s="3"/>
     </row>
     <row r="168" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B168" s="3"/>
     </row>
     <row r="169" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B169" s="2" t="s">
         <v>82</v>
@@ -2722,45 +2718,45 @@
     </row>
     <row r="170" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B172" s="3"/>
     </row>
     <row r="173" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B175" s="2" t="s">
         <v>54</v>
@@ -2768,117 +2764,117 @@
     </row>
     <row r="176" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B177" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B178" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B179" s="2" t="s">
         <v>252</v>
-      </c>
-      <c r="B179" s="2" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B180" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="B180" s="2" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B181" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="B181" s="2" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B182" s="3"/>
     </row>
     <row r="183" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B183" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="B183" s="2" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B184" s="2" t="s">
         <v>261</v>
-      </c>
-      <c r="B184" s="2" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B185" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="B185" s="2" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B186" s="2" t="s">
         <v>265</v>
-      </c>
-      <c r="B186" s="2" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B187" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="B187" s="2" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="B188" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="B188" s="2" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B189" s="2" t="s">
         <v>271</v>
-      </c>
-      <c r="B189" s="2" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B190" s="2" t="s">
         <v>31</v>
@@ -2886,291 +2882,291 @@
     </row>
     <row r="191" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B191" s="3"/>
     </row>
     <row r="192" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B192" s="3"/>
     </row>
     <row r="193" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B193" s="3"/>
     </row>
     <row r="194" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B194" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="B194" s="2" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="B195" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="B195" s="2" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B196" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="B196" s="2" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B197" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="B197" s="2" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B198" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="B198" s="2" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B199" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="B199" s="2" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B200" s="3"/>
     </row>
     <row r="201" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B201" s="3"/>
     </row>
     <row r="202" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A202" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B202" s="3"/>
+    </row>
+    <row r="203" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A203" s="6" t="s">
         <v>291</v>
-      </c>
-      <c r="B202" s="3"/>
-    </row>
-    <row r="203" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A203" s="6" t="s">
-        <v>292</v>
       </c>
       <c r="B203" s="7"/>
     </row>
     <row r="204" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B204" s="3"/>
     </row>
     <row r="205" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B205" s="3"/>
     </row>
     <row r="206" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B206" s="3"/>
     </row>
     <row r="207" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A207" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B207" s="3"/>
     </row>
     <row r="208" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B208" s="3"/>
     </row>
     <row r="209" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A209" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B209" s="3"/>
     </row>
     <row r="210" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B210" s="3"/>
     </row>
     <row r="211" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B211" s="3"/>
     </row>
     <row r="212" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B212" s="3"/>
+    </row>
+    <row r="213" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A213" s="6" t="s">
         <v>301</v>
-      </c>
-      <c r="B212" s="3"/>
-    </row>
-    <row r="213" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A213" s="6" t="s">
-        <v>302</v>
       </c>
       <c r="B213" s="7"/>
     </row>
     <row r="214" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B214" s="3"/>
     </row>
     <row r="215" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B215" s="3"/>
     </row>
     <row r="216" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A216" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B216" s="3"/>
+    </row>
+    <row r="217" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A217" s="6" t="s">
         <v>305</v>
-      </c>
-      <c r="B216" s="3"/>
-    </row>
-    <row r="217" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A217" s="6" t="s">
-        <v>306</v>
       </c>
       <c r="B217" s="7"/>
     </row>
     <row r="218" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A218" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B220" s="2" t="s">
         <v>309</v>
-      </c>
-      <c r="B220" s="2" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A221" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B221" s="2" t="s">
         <v>311</v>
-      </c>
-      <c r="B221" s="2" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A223" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="B223" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="B223" s="2" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A224" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="B224" s="2" t="s">
         <v>315</v>
-      </c>
-      <c r="B224" s="2" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A226" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B226" s="3"/>
     </row>
     <row r="227" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A227" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B227" s="3"/>
     </row>
     <row r="228" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A228" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B228" s="3"/>
     </row>
     <row r="229" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A229" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B229" s="2" t="s">
         <v>320</v>
-      </c>
-      <c r="B229" s="2" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B230" s="2" t="s">
         <v>322</v>
-      </c>
-      <c r="B230" s="2" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A231" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B231" s="3"/>
     </row>
     <row r="232" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B232" s="3"/>
+    </row>
+    <row r="233" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A233" s="6" t="s">
         <v>325</v>
-      </c>
-      <c r="B232" s="3"/>
-    </row>
-    <row r="233" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A233" s="6" t="s">
-        <v>326</v>
       </c>
       <c r="B233" s="7"/>
     </row>
@@ -3184,7 +3180,7 @@
     </row>
     <row r="235" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A235" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B235" s="2" t="s">
         <v>39</v>
@@ -3192,167 +3188,167 @@
     </row>
     <row r="236" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A236" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B236" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="B236" s="2" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A237" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B237" s="3"/>
+    </row>
+    <row r="238" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A238" s="6" t="s">
         <v>330</v>
-      </c>
-      <c r="B237" s="3"/>
-    </row>
-    <row r="238" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A238" s="6" t="s">
-        <v>331</v>
       </c>
       <c r="B238" s="7"/>
     </row>
     <row r="239" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A239" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B239" s="3"/>
     </row>
     <row r="240" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A240" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B240" s="3"/>
     </row>
     <row r="241" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A241" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B241" s="3"/>
     </row>
     <row r="242" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A242" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B242" s="3"/>
     </row>
     <row r="243" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A243" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B243" s="3"/>
     </row>
     <row r="244" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A244" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B244" s="3"/>
     </row>
     <row r="245" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A245" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B245" s="3"/>
     </row>
     <row r="246" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A246" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B246" s="3"/>
     </row>
     <row r="247" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A247" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B247" s="3"/>
     </row>
     <row r="248" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A248" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B248" s="3"/>
     </row>
     <row r="249" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A249" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B249" s="3"/>
+    </row>
+    <row r="250" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A250" s="5" t="s">
         <v>342</v>
       </c>
-      <c r="B249" s="3"/>
-    </row>
-    <row r="250" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A250" s="5" t="s">
+      <c r="B250" s="3"/>
+    </row>
+    <row r="251" spans="1:2" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A251" s="5" t="s">
         <v>343</v>
-      </c>
-      <c r="B250" s="3"/>
-    </row>
-    <row r="251" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A251" s="5" t="s">
-        <v>344</v>
       </c>
       <c r="B251" s="3"/>
     </row>
     <row r="252" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A252" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B252" s="3"/>
     </row>
     <row r="253" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A253" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B253" s="3"/>
     </row>
     <row r="254" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A254" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B254" s="3"/>
     </row>
     <row r="255" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A255" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B255" s="3"/>
     </row>
     <row r="256" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A256" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B256" s="3"/>
     </row>
     <row r="257" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A257" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B257" s="3"/>
     </row>
     <row r="258" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A258" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B258" s="3"/>
     </row>
     <row r="259" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A259" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B259" s="3"/>
     </row>
     <row r="260" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A260" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B260" s="3"/>
     </row>
     <row r="261" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A261" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A262" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B262" s="2" t="s">
         <v>46</v>
@@ -3360,7 +3356,7 @@
     </row>
     <row r="263" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A263" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B263" s="2" t="s">
         <v>42</v>
@@ -3368,7 +3364,7 @@
     </row>
     <row r="264" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A264" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B264" s="2" t="s">
         <v>54</v>
@@ -3376,26 +3372,26 @@
     </row>
     <row r="265" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A265" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A266" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A267" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -3408,18 +3404,18 @@
     <mergeCell ref="A233:B233"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A111" r:id="rId1" display="http://lk.u.rw/" xr:uid="{B9E4BD0B-91D2-4FD4-9ABD-871EA312D809}"/>
-    <hyperlink ref="A161" r:id="rId2" display="http://lcomp.pr/" xr:uid="{403ECDDB-6691-49E3-9EF6-E88F468B06EA}"/>
-    <hyperlink ref="A163" r:id="rId3" display="http://lcomp.d.pr/" xr:uid="{C5A579A5-1E24-40B0-BF5B-A5C99625F4F7}"/>
-    <hyperlink ref="A165" r:id="rId4" display="http://acomp.pr/" xr:uid="{D7168372-AEDD-442E-9C6F-E16ABCE87316}"/>
-    <hyperlink ref="A188" r:id="rId5" display="http://u.pr/" xr:uid="{6FFAF3D3-FD95-4F54-98D3-1A67154C054E}"/>
-    <hyperlink ref="A195" r:id="rId6" display="http://l.pr/" xr:uid="{271A868E-8ED8-40B2-AAE4-23CC6B0BCAF5}"/>
-    <hyperlink ref="A198" r:id="rId7" display="http://d.pr/" xr:uid="{BC8E8F1B-AB78-46FD-A8B2-5C67E741EDD3}"/>
-    <hyperlink ref="A223" r:id="rId8" display="http://length.cv/" xr:uid="{AE5C3911-1B65-45B6-B34F-DE3F5BB36030}"/>
-    <hyperlink ref="A224" r:id="rId9" display="http://length.sd/" xr:uid="{521335C9-74F6-4BBF-B444-AF8F6173B0E5}"/>
-    <hyperlink ref="A226" r:id="rId10" display="http://wgt.mt/" xr:uid="{DC7FFAC2-4E74-41F8-A4F0-D8BB639F74C4}"/>
-    <hyperlink ref="A250" r:id="rId11" display="http://ypr.lb/" xr:uid="{AFEEA483-6DF1-4C4B-86A0-DA30CB0CC74F}"/>
-    <hyperlink ref="A251" r:id="rId12" display="http://total.lb/" xr:uid="{577BCCC4-265F-4A53-9F25-16E302A48204}"/>
+    <hyperlink ref="A111" r:id="rId1" display="http://lk.u.rw/"/>
+    <hyperlink ref="A161" r:id="rId2" display="http://lcomp.pr/"/>
+    <hyperlink ref="A163" r:id="rId3" display="http://lcomp.d.pr/"/>
+    <hyperlink ref="A165" r:id="rId4" display="http://acomp.pr/"/>
+    <hyperlink ref="A188" r:id="rId5" display="http://u.pr/"/>
+    <hyperlink ref="A195" r:id="rId6" display="http://l.pr/"/>
+    <hyperlink ref="A198" r:id="rId7" display="http://d.pr/"/>
+    <hyperlink ref="A223" r:id="rId8" display="http://length.cv/"/>
+    <hyperlink ref="A224" r:id="rId9" display="http://length.sd/"/>
+    <hyperlink ref="A226" r:id="rId10" display="http://wgt.mt/"/>
+    <hyperlink ref="A250" r:id="rId11" display="http://ypr.lb/"/>
+    <hyperlink ref="A251" r:id="rId12" display="http://total.lb/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>

</xml_diff>

<commit_message>
update naming conventions for labels in SS3 and BAM; add new conversion sheet for FIMS naming based on recent example
</commit_message>
<xml_diff>
--- a/inst/resources/bam_var_names.xlsx
+++ b/inst/resources/bam_var_names.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="405">
   <si>
     <t>module_name</t>
   </si>
@@ -777,9 +777,6 @@
     <t>lcomp.ob</t>
   </si>
   <si>
-    <t>length_composition_observed</t>
-  </si>
-  <si>
     <t>lcomp.pr</t>
   </si>
   <si>
@@ -789,9 +786,6 @@
     <t>lcomp.D.ob</t>
   </si>
   <si>
-    <t>length_composition_discard_observed</t>
-  </si>
-  <si>
     <t>lcomp.D.pr</t>
   </si>
   <si>
@@ -801,9 +795,6 @@
     <t>acomp.ob</t>
   </si>
   <si>
-    <t>age_composition_observed</t>
-  </si>
-  <si>
     <t>acomp.pr</t>
   </si>
   <si>
@@ -909,21 +900,12 @@
     <t>U.ob</t>
   </si>
   <si>
-    <t>cpue_observed</t>
-  </si>
-  <si>
     <t>U.pr</t>
   </si>
   <si>
-    <t>cpue_predicted</t>
-  </si>
-  <si>
     <t>cv.U</t>
   </si>
   <si>
-    <t>cpue_cv</t>
-  </si>
-  <si>
     <t>q.rate.mult</t>
   </si>
   <si>
@@ -939,9 +921,6 @@
     <t>L.ob</t>
   </si>
   <si>
-    <t>landings_observed</t>
-  </si>
-  <si>
     <t>L.pr</t>
   </si>
   <si>
@@ -957,9 +936,6 @@
     <t>D.ob</t>
   </si>
   <si>
-    <t>discard_observed</t>
-  </si>
-  <si>
     <t>D.pr</t>
   </si>
   <si>
@@ -1210,6 +1186,54 @@
   </si>
   <si>
     <t>proj.N.age</t>
+  </si>
+  <si>
+    <t>length_composition_expected</t>
+  </si>
+  <si>
+    <t>length_composition_discard_expected</t>
+  </si>
+  <si>
+    <t>age_composition_expected</t>
+  </si>
+  <si>
+    <t>landings_expected</t>
+  </si>
+  <si>
+    <t>discard_expected</t>
+  </si>
+  <si>
+    <t>indices_expected</t>
+  </si>
+  <si>
+    <t>indices_predicted</t>
+  </si>
+  <si>
+    <t>indices_cv</t>
+  </si>
+  <si>
+    <t>virgin_recruitment</t>
+  </si>
+  <si>
+    <t>recruitment_lag</t>
+  </si>
+  <si>
+    <t>log_abundance_deviations</t>
+  </si>
+  <si>
+    <t>fishing_mortality_discards</t>
+  </si>
+  <si>
+    <t>length_composition</t>
+  </si>
+  <si>
+    <t>length_composition_discards</t>
+  </si>
+  <si>
+    <t>age_composition</t>
+  </si>
+  <si>
+    <t>ypr</t>
   </si>
 </sst>
 </file>
@@ -1564,11 +1588,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="C164" sqref="C164"/>
+    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
+      <selection activeCell="C272" sqref="C272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.90625" customWidth="1"/>
+    <col min="2" max="2" width="19.1796875" customWidth="1"/>
+    <col min="3" max="3" width="31.90625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -2083,6 +2112,9 @@
       <c r="B50" t="s">
         <v>72</v>
       </c>
+      <c r="C50" t="s">
+        <v>397</v>
+      </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
@@ -2090,6 +2122,9 @@
       </c>
       <c r="B51" t="s">
         <v>73</v>
+      </c>
+      <c r="C51" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -3108,6 +3143,9 @@
       <c r="B156" t="s">
         <v>213</v>
       </c>
+      <c r="C156" t="s">
+        <v>399</v>
+      </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
@@ -3116,6 +3154,9 @@
       <c r="B157" t="s">
         <v>213</v>
       </c>
+      <c r="C157" t="s">
+        <v>399</v>
+      </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
@@ -3220,6 +3261,9 @@
       <c r="B167" t="s">
         <v>233</v>
       </c>
+      <c r="C167" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B168" t="s">
@@ -3315,65 +3359,71 @@
         <v>251</v>
       </c>
       <c r="C181" t="s">
-        <v>252</v>
+        <v>389</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B182" t="s">
+        <v>252</v>
+      </c>
+      <c r="C182" t="s">
         <v>253</v>
-      </c>
-      <c r="C182" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B183" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C183" t="s">
-        <v>256</v>
+        <v>390</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B184" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C184" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B185" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C185" t="s">
-        <v>260</v>
+        <v>391</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B186" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C186" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B187" t="s">
-        <v>263</v>
+        <v>260</v>
+      </c>
+      <c r="C187" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B188" t="s">
-        <v>264</v>
+        <v>261</v>
+      </c>
+      <c r="C188" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B189" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.35">
@@ -3381,7 +3431,7 @@
         <v>36</v>
       </c>
       <c r="B190" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C190" t="s">
         <v>94</v>
@@ -3392,10 +3442,10 @@
         <v>36</v>
       </c>
       <c r="B191" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C191" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.35">
@@ -3403,7 +3453,7 @@
         <v>36</v>
       </c>
       <c r="B192" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C192" t="s">
         <v>223</v>
@@ -3414,7 +3464,10 @@
         <v>36</v>
       </c>
       <c r="B193" t="s">
-        <v>271</v>
+        <v>268</v>
+      </c>
+      <c r="C193" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.35">
@@ -3422,10 +3475,10 @@
         <v>36</v>
       </c>
       <c r="B194" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C194" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.35">
@@ -3433,7 +3486,7 @@
         <v>36</v>
       </c>
       <c r="B195" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C195" t="s">
         <v>216</v>
@@ -3444,7 +3497,7 @@
         <v>36</v>
       </c>
       <c r="B196" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C196" t="s">
         <v>63</v>
@@ -3455,10 +3508,10 @@
         <v>36</v>
       </c>
       <c r="B197" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C197" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.35">
@@ -3466,10 +3519,10 @@
         <v>36</v>
       </c>
       <c r="B198" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C198" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.35">
@@ -3477,10 +3530,10 @@
         <v>36</v>
       </c>
       <c r="B199" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C199" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.35">
@@ -3488,10 +3541,10 @@
         <v>36</v>
       </c>
       <c r="B200" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C200" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.35">
@@ -3499,10 +3552,10 @@
         <v>36</v>
       </c>
       <c r="B201" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C201" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.35">
@@ -3510,10 +3563,10 @@
         <v>36</v>
       </c>
       <c r="B202" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C202" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.35">
@@ -3521,7 +3574,7 @@
         <v>36</v>
       </c>
       <c r="B203" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.35">
@@ -3529,7 +3582,7 @@
         <v>36</v>
       </c>
       <c r="B204" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C204" t="s">
         <v>180</v>
@@ -3540,10 +3593,10 @@
         <v>36</v>
       </c>
       <c r="B205" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C205" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.35">
@@ -3551,7 +3604,7 @@
         <v>36</v>
       </c>
       <c r="B206" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C206" t="s">
         <v>182</v>
@@ -3562,10 +3615,10 @@
         <v>36</v>
       </c>
       <c r="B207" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C207" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.35">
@@ -3573,10 +3626,10 @@
         <v>36</v>
       </c>
       <c r="B208" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C208" t="s">
-        <v>296</v>
+        <v>394</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.35">
@@ -3584,10 +3637,10 @@
         <v>36</v>
       </c>
       <c r="B209" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C209" t="s">
-        <v>298</v>
+        <v>395</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.35">
@@ -3595,10 +3648,10 @@
         <v>36</v>
       </c>
       <c r="B210" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="C210" t="s">
-        <v>300</v>
+        <v>396</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.35">
@@ -3606,7 +3659,7 @@
         <v>36</v>
       </c>
       <c r="B211" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="C211" t="s">
         <v>38</v>
@@ -3617,7 +3670,7 @@
         <v>36</v>
       </c>
       <c r="B212" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.35">
@@ -3625,7 +3678,7 @@
         <v>36</v>
       </c>
       <c r="B213" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.35">
@@ -3633,7 +3686,7 @@
         <v>36</v>
       </c>
       <c r="B214" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.35">
@@ -3641,10 +3694,10 @@
         <v>36</v>
       </c>
       <c r="B215" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="C215" t="s">
-        <v>306</v>
+        <v>392</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.35">
@@ -3652,10 +3705,10 @@
         <v>36</v>
       </c>
       <c r="B216" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="C216" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.35">
@@ -3663,10 +3716,10 @@
         <v>36</v>
       </c>
       <c r="B217" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="C217" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.35">
@@ -3674,10 +3727,10 @@
         <v>36</v>
       </c>
       <c r="B218" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="C218" t="s">
-        <v>312</v>
+        <v>393</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.35">
@@ -3685,10 +3738,10 @@
         <v>36</v>
       </c>
       <c r="B219" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="C219" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.35">
@@ -3696,40 +3749,40 @@
         <v>36</v>
       </c>
       <c r="B220" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="C220" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B221" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B222" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B223" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B224" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B225" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B226" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.35">
@@ -3737,7 +3790,10 @@
         <v>36</v>
       </c>
       <c r="B227" t="s">
-        <v>323</v>
+        <v>315</v>
+      </c>
+      <c r="C227" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.35">
@@ -3745,7 +3801,10 @@
         <v>36</v>
       </c>
       <c r="B228" t="s">
-        <v>324</v>
+        <v>316</v>
+      </c>
+      <c r="C228" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.35">
@@ -3753,7 +3812,10 @@
         <v>36</v>
       </c>
       <c r="B229" t="s">
-        <v>325</v>
+        <v>317</v>
+      </c>
+      <c r="C229" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.35">
@@ -3761,7 +3823,7 @@
         <v>36</v>
       </c>
       <c r="B230" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.35">
@@ -3769,7 +3831,7 @@
         <v>36</v>
       </c>
       <c r="B231" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.35">
@@ -3777,7 +3839,7 @@
         <v>36</v>
       </c>
       <c r="B232" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.35">
@@ -3785,7 +3847,7 @@
         <v>36</v>
       </c>
       <c r="B233" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.35">
@@ -3793,7 +3855,7 @@
         <v>36</v>
       </c>
       <c r="B234" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.35">
@@ -3801,7 +3863,7 @@
         <v>36</v>
       </c>
       <c r="B235" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.35">
@@ -3809,7 +3871,7 @@
         <v>36</v>
       </c>
       <c r="B236" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.35">
@@ -3817,7 +3879,7 @@
         <v>36</v>
       </c>
       <c r="B237" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.35">
@@ -3825,15 +3887,15 @@
         <v>36</v>
       </c>
       <c r="B238" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B239" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="C239" t="s">
         <v>180</v>
@@ -3841,35 +3903,35 @@
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B240" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="C240" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B241" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C241" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="B242" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="C242" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.35">
@@ -3888,10 +3950,10 @@
         <v>236</v>
       </c>
       <c r="B244" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="C244" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.35">
@@ -3899,10 +3961,10 @@
         <v>236</v>
       </c>
       <c r="B245" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="C245" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.35">
@@ -3921,7 +3983,7 @@
         <v>236</v>
       </c>
       <c r="B247" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.35">
@@ -3929,7 +3991,7 @@
         <v>236</v>
       </c>
       <c r="B248" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.35">
@@ -3937,7 +3999,7 @@
         <v>236</v>
       </c>
       <c r="B249" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.35">
@@ -3945,10 +4007,10 @@
         <v>236</v>
       </c>
       <c r="B250" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="C250" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.35">
@@ -3956,10 +4018,10 @@
         <v>236</v>
       </c>
       <c r="B251" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="C251" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.35">
@@ -3967,7 +4029,7 @@
         <v>236</v>
       </c>
       <c r="B252" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.35">
@@ -3975,7 +4037,7 @@
         <v>236</v>
       </c>
       <c r="B253" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.35">
@@ -3983,7 +4045,7 @@
         <v>236</v>
       </c>
       <c r="B254" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.35">
@@ -3991,7 +4053,7 @@
         <v>236</v>
       </c>
       <c r="B255" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="C255" t="s">
         <v>11</v>
@@ -4002,10 +4064,10 @@
         <v>236</v>
       </c>
       <c r="B256" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="C256" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.35">
@@ -4013,10 +4075,10 @@
         <v>236</v>
       </c>
       <c r="B257" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="C257" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.35">
@@ -4024,7 +4086,7 @@
         <v>236</v>
       </c>
       <c r="B258" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.35">
@@ -4032,170 +4094,179 @@
         <v>236</v>
       </c>
       <c r="B259" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="B260" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="B261" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="B262" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="B263" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="B264" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="B265" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="B266" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
+        <v>355</v>
+      </c>
+      <c r="B267" t="s">
         <v>363</v>
-      </c>
-      <c r="B267" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="B268" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="B269" t="s">
-        <v>374</v>
+        <v>366</v>
+      </c>
+      <c r="C269" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="B270" t="s">
-        <v>375</v>
+        <v>367</v>
+      </c>
+      <c r="C270" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="B271" t="s">
-        <v>376</v>
+        <v>368</v>
+      </c>
+      <c r="C271" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="B272" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="B273" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B274" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B275" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B276" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B277" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B278" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B279" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B280" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="B281" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="B282" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="C282" t="s">
         <v>223</v>
@@ -4203,10 +4274,10 @@
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="B283" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="C283" t="s">
         <v>55</v>
@@ -4214,10 +4285,10 @@
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="B284" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="C284" t="s">
         <v>51</v>
@@ -4225,10 +4296,10 @@
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="B285" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="C285" t="s">
         <v>63</v>
@@ -4236,21 +4307,21 @@
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="B286" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="C286" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="B287" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="C287" t="s">
         <v>180</v>
@@ -4258,10 +4329,10 @@
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="B288" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="C288" t="s">
         <v>216</v>

</xml_diff>

<commit_message>
fix naming conventions for spr
</commit_message>
<xml_diff>
--- a/inst/resources/bam_var_names.xlsx
+++ b/inst/resources/bam_var_names.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="406">
   <si>
     <t>module_name</t>
   </si>
@@ -1234,6 +1234,9 @@
   </si>
   <si>
     <t>ypr</t>
+  </si>
+  <si>
+    <t>f_spr</t>
   </si>
 </sst>
 </file>
@@ -1589,7 +1592,7 @@
   <dimension ref="A1:C288"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
-      <selection activeCell="C272" sqref="C272"/>
+      <selection activeCell="C269" sqref="C269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3576,6 +3579,9 @@
       <c r="B203" t="s">
         <v>285</v>
       </c>
+      <c r="C203" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
@@ -4104,6 +4110,9 @@
       <c r="B260" t="s">
         <v>356</v>
       </c>
+      <c r="C260" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
@@ -4112,6 +4121,9 @@
       <c r="B261" t="s">
         <v>357</v>
       </c>
+      <c r="C261" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
@@ -4120,6 +4132,9 @@
       <c r="B262" t="s">
         <v>358</v>
       </c>
+      <c r="C262" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
@@ -4128,6 +4143,9 @@
       <c r="B263" t="s">
         <v>359</v>
       </c>
+      <c r="C263" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
@@ -4136,6 +4154,9 @@
       <c r="B264" t="s">
         <v>360</v>
       </c>
+      <c r="C264" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
@@ -4144,6 +4165,9 @@
       <c r="B265" t="s">
         <v>361</v>
       </c>
+      <c r="C265" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
@@ -4152,6 +4176,9 @@
       <c r="B266" t="s">
         <v>362</v>
       </c>
+      <c r="C266" t="s">
+        <v>333</v>
+      </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
@@ -4160,6 +4187,9 @@
       <c r="B267" t="s">
         <v>363</v>
       </c>
+      <c r="C267" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
@@ -4167,6 +4197,9 @@
       </c>
       <c r="B268" t="s">
         <v>365</v>
+      </c>
+      <c r="C268" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
fix issues in conout with BAM and adjusting bam var names and improving them
</commit_message>
<xml_diff>
--- a/inst/resources/bam_var_names.xlsx
+++ b/inst/resources/bam_var_names.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="496">
   <si>
     <t>module_name</t>
   </si>
@@ -1237,6 +1237,276 @@
   </si>
   <si>
     <t>f_spr</t>
+  </si>
+  <si>
+    <t>l.klb</t>
+  </si>
+  <si>
+    <t>l.knum</t>
+  </si>
+  <si>
+    <t>d.klb</t>
+  </si>
+  <si>
+    <t>d.knum</t>
+  </si>
+  <si>
+    <t>fec_batches</t>
+  </si>
+  <si>
+    <t>fec_scale</t>
+  </si>
+  <si>
+    <t>catchability_beta</t>
+  </si>
+  <si>
+    <t>q_DD_B0_4plus</t>
+  </si>
+  <si>
+    <t>rec_mu_end</t>
+  </si>
+  <si>
+    <t>R_sigma_logdevs</t>
+  </si>
+  <si>
+    <t>R_sigma_par</t>
+  </si>
+  <si>
+    <t>Dmort_GR</t>
+  </si>
+  <si>
+    <t>Dmort_cP</t>
+  </si>
+  <si>
+    <t>lk_total</t>
+  </si>
+  <si>
+    <t>lk_U</t>
+  </si>
+  <si>
+    <t>lk_L</t>
+  </si>
+  <si>
+    <t>lk_D</t>
+  </si>
+  <si>
+    <t>lk_lenc</t>
+  </si>
+  <si>
+    <t>lk_agec</t>
+  </si>
+  <si>
+    <t>lk_priors</t>
+  </si>
+  <si>
+    <t>lk_SRfit</t>
+  </si>
+  <si>
+    <t>lk_SRearly</t>
+  </si>
+  <si>
+    <t>lk_SRend</t>
+  </si>
+  <si>
+    <t>w_lc</t>
+  </si>
+  <si>
+    <t>w_ac</t>
+  </si>
+  <si>
+    <t>w_U</t>
+  </si>
+  <si>
+    <t>lk_unwgt_data</t>
+  </si>
+  <si>
+    <t>lk_lenc_D</t>
+  </si>
+  <si>
+    <t>lk_agec_Mcvt</t>
+  </si>
+  <si>
+    <t>lk_U_RW</t>
+  </si>
+  <si>
+    <t>w_lc_D</t>
+  </si>
+  <si>
+    <t>w_ac_Mcvt</t>
+  </si>
+  <si>
+    <t>w_R</t>
+  </si>
+  <si>
+    <t>w_R_init</t>
+  </si>
+  <si>
+    <t>w_R_end</t>
+  </si>
+  <si>
+    <t>gradient_max</t>
+  </si>
+  <si>
+    <t>len_cT_mm</t>
+  </si>
+  <si>
+    <t>len_D_mm</t>
+  </si>
+  <si>
+    <t>wgt_cP_klb</t>
+  </si>
+  <si>
+    <t>wgt_cT_klb</t>
+  </si>
+  <si>
+    <t>wgt_D_klb</t>
+  </si>
+  <si>
+    <t>sel_v</t>
+  </si>
+  <si>
+    <t>sel_v_Mcvt</t>
+  </si>
+  <si>
+    <t>sel_m</t>
+  </si>
+  <si>
+    <t>sel_m_D</t>
+  </si>
+  <si>
+    <t>sdnr_U</t>
+  </si>
+  <si>
+    <t>q_DD_mult</t>
+  </si>
+  <si>
+    <t>cl_D_release</t>
+  </si>
+  <si>
+    <t>cl_Dosed_release</t>
+  </si>
+  <si>
+    <t>cp_D_release</t>
+  </si>
+  <si>
+    <t>cp_Dosed_release</t>
+  </si>
+  <si>
+    <t>hb_D_release</t>
+  </si>
+  <si>
+    <t>mrip_D_release</t>
+  </si>
+  <si>
+    <t>acomp_Mcvt_n</t>
+  </si>
+  <si>
+    <t>lcomp_nfish</t>
+  </si>
+  <si>
+    <t>lcomp_D_nfish</t>
+  </si>
+  <si>
+    <t>acomp_nfish</t>
+  </si>
+  <si>
+    <t>acomp_Mcvt_nfish</t>
+  </si>
+  <si>
+    <t>lcomp_neff</t>
+  </si>
+  <si>
+    <t>lcomp_D_neff</t>
+  </si>
+  <si>
+    <t>acomp_neff</t>
+  </si>
+  <si>
+    <t>acomp_Mcvt_neff</t>
+  </si>
+  <si>
+    <t>wgt_mt</t>
+  </si>
+  <si>
+    <t>fecundity_scaled</t>
+  </si>
+  <si>
+    <t>reprod_MatFemB</t>
+  </si>
+  <si>
+    <t>Nage_eq_init</t>
+  </si>
+  <si>
+    <t>total_lb</t>
+  </si>
+  <si>
+    <t>Lw_total</t>
+  </si>
+  <si>
+    <t>Dw_total</t>
+  </si>
+  <si>
+    <t>Ln_total</t>
+  </si>
+  <si>
+    <t>Dn_total</t>
+  </si>
+  <si>
+    <t>error_mat</t>
+  </si>
+  <si>
+    <t>sel_v_wgted_L</t>
+  </si>
+  <si>
+    <t>log_F_dev_cP</t>
+  </si>
+  <si>
+    <t>log_F_dev_cT</t>
+  </si>
+  <si>
+    <t>sel_v_wgted_D</t>
+  </si>
+  <si>
+    <t>sel_v_wgted_tot</t>
+  </si>
+  <si>
+    <t>q_DD_B_4plus</t>
+  </si>
+  <si>
+    <t>q_RW_log_dev</t>
+  </si>
+  <si>
+    <t>wgt_wgted_L_klb</t>
+  </si>
+  <si>
+    <t>wgt_wgted_D_klb</t>
+  </si>
+  <si>
+    <t>log_Nage2plus_plus.init_dev</t>
+  </si>
+  <si>
+    <t>rstyr.r0</t>
+  </si>
+  <si>
+    <t>recruitment_start_year_R0</t>
+  </si>
+  <si>
+    <t>mean.r0</t>
+  </si>
+  <si>
+    <t>mean_R0</t>
+  </si>
+  <si>
+    <t>ssbstyr.ssb0</t>
+  </si>
+  <si>
+    <t>spawning_biomass_start_year_spawning_biomass0</t>
+  </si>
+  <si>
+    <t>f.prop.d</t>
+  </si>
+  <si>
+    <t>f_prop_d</t>
   </si>
 </sst>
 </file>
@@ -1589,10 +1859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C288"/>
+  <dimension ref="A1:C296"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
-      <selection activeCell="C269" sqref="C269"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1754,6 +2024,9 @@
       <c r="B15" t="s">
         <v>24</v>
       </c>
+      <c r="C15" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -1761,6 +2034,9 @@
       </c>
       <c r="B16" t="s">
         <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1877,6 +2153,9 @@
       <c r="B27" t="s">
         <v>39</v>
       </c>
+      <c r="C27" t="s">
+        <v>412</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
@@ -1885,16 +2164,19 @@
       <c r="B28" t="s">
         <v>40</v>
       </c>
+      <c r="C28" t="s">
+        <v>413</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>494</v>
       </c>
       <c r="C29" t="s">
-        <v>42</v>
+        <v>495</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -1902,7 +2184,7 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C30" t="s">
         <v>42</v>
@@ -1913,7 +2195,7 @@
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C31" t="s">
         <v>42</v>
@@ -1924,7 +2206,7 @@
         <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C32" t="s">
         <v>42</v>
@@ -1935,10 +2217,10 @@
         <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C33" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
@@ -1946,10 +2228,10 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C34" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -1957,15 +2239,15 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C35" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="B36" t="s">
         <v>50</v>
@@ -1976,13 +2258,13 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C37" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
@@ -1990,15 +2272,15 @@
         <v>3</v>
       </c>
       <c r="B38" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C38" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="B39" t="s">
         <v>54</v>
@@ -2009,13 +2291,13 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C40" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
@@ -2023,10 +2305,10 @@
         <v>3</v>
       </c>
       <c r="B41" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C41" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
@@ -2034,10 +2316,10 @@
         <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>60</v>
+        <v>492</v>
       </c>
       <c r="C42" t="s">
-        <v>61</v>
+        <v>493</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
@@ -2045,10 +2327,10 @@
         <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C43" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -2056,10 +2338,10 @@
         <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>64</v>
+        <v>488</v>
       </c>
       <c r="C44" t="s">
-        <v>65</v>
+        <v>489</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
@@ -2067,7 +2349,10 @@
         <v>3</v>
       </c>
       <c r="B45" t="s">
-        <v>66</v>
+        <v>60</v>
+      </c>
+      <c r="C45" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
@@ -2075,7 +2360,10 @@
         <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>67</v>
+        <v>490</v>
+      </c>
+      <c r="C46" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
@@ -2083,7 +2371,10 @@
         <v>3</v>
       </c>
       <c r="B47" t="s">
-        <v>68</v>
+        <v>62</v>
+      </c>
+      <c r="C47" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
@@ -2091,10 +2382,10 @@
         <v>3</v>
       </c>
       <c r="B48" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C48" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
@@ -2102,10 +2393,10 @@
         <v>3</v>
       </c>
       <c r="B49" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C49" t="s">
-        <v>63</v>
+        <v>414</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -2113,10 +2404,10 @@
         <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C50" t="s">
-        <v>397</v>
+        <v>415</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
@@ -2124,10 +2415,10 @@
         <v>3</v>
       </c>
       <c r="B51" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C51" t="s">
-        <v>398</v>
+        <v>416</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -2135,10 +2426,10 @@
         <v>3</v>
       </c>
       <c r="B52" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C52" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
@@ -2146,10 +2437,10 @@
         <v>3</v>
       </c>
       <c r="B53" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C53" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
@@ -2157,10 +2448,10 @@
         <v>3</v>
       </c>
       <c r="B54" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C54" t="s">
-        <v>79</v>
+        <v>397</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
@@ -2168,10 +2459,10 @@
         <v>3</v>
       </c>
       <c r="B55" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C55" t="s">
-        <v>81</v>
+        <v>398</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
@@ -2179,10 +2470,10 @@
         <v>3</v>
       </c>
       <c r="B56" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C56" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
@@ -2190,10 +2481,10 @@
         <v>3</v>
       </c>
       <c r="B57" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C57" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
@@ -2201,10 +2492,10 @@
         <v>3</v>
       </c>
       <c r="B58" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C58" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
@@ -2212,10 +2503,10 @@
         <v>3</v>
       </c>
       <c r="B59" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C59" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
@@ -2223,10 +2514,10 @@
         <v>3</v>
       </c>
       <c r="B60" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C60" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
@@ -2234,10 +2525,10 @@
         <v>3</v>
       </c>
       <c r="B61" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C61" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
@@ -2245,10 +2536,10 @@
         <v>3</v>
       </c>
       <c r="B62" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C62" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
@@ -2256,10 +2547,10 @@
         <v>3</v>
       </c>
       <c r="B63" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C63" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
@@ -2267,10 +2558,10 @@
         <v>3</v>
       </c>
       <c r="B64" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C64" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
@@ -2278,10 +2569,10 @@
         <v>3</v>
       </c>
       <c r="B65" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C65" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
@@ -2289,21 +2580,21 @@
         <v>3</v>
       </c>
       <c r="B66" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C66" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>103</v>
+        <v>3</v>
       </c>
       <c r="B67" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C67" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
@@ -2311,21 +2602,21 @@
         <v>3</v>
       </c>
       <c r="B68" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C68" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>103</v>
+        <v>3</v>
       </c>
       <c r="B69" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C69" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
@@ -2333,10 +2624,10 @@
         <v>3</v>
       </c>
       <c r="B70" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C70" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
@@ -2344,10 +2635,10 @@
         <v>103</v>
       </c>
       <c r="B71" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C71" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
@@ -2355,10 +2646,10 @@
         <v>3</v>
       </c>
       <c r="B72" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C72" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
@@ -2366,10 +2657,10 @@
         <v>103</v>
       </c>
       <c r="B73" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C73" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
@@ -2377,10 +2668,10 @@
         <v>3</v>
       </c>
       <c r="B74" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C74" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
@@ -2388,10 +2679,10 @@
         <v>103</v>
       </c>
       <c r="B75" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C75" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
@@ -2399,10 +2690,10 @@
         <v>3</v>
       </c>
       <c r="B76" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C76" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
@@ -2410,10 +2701,10 @@
         <v>103</v>
       </c>
       <c r="B77" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C77" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
@@ -2421,10 +2712,10 @@
         <v>3</v>
       </c>
       <c r="B78" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C78" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
@@ -2432,10 +2723,10 @@
         <v>103</v>
       </c>
       <c r="B79" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C79" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
@@ -2443,23 +2734,32 @@
         <v>3</v>
       </c>
       <c r="B80" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C80" t="s">
-        <v>29</v>
+        <v>113</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>3</v>
+        <v>103</v>
       </c>
       <c r="B81" t="s">
-        <v>116</v>
+        <v>112</v>
+      </c>
+      <c r="C81" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>3</v>
+      </c>
       <c r="B82" t="s">
-        <v>117</v>
+        <v>114</v>
+      </c>
+      <c r="C82" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
@@ -2467,43 +2767,43 @@
         <v>103</v>
       </c>
       <c r="B83" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C83" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>103</v>
+        <v>3</v>
       </c>
       <c r="B84" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C84" t="s">
-        <v>120</v>
+        <v>29</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>103</v>
+        <v>3</v>
       </c>
       <c r="B85" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C85" t="s">
-        <v>121</v>
+        <v>417</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>103</v>
+        <v>3</v>
       </c>
       <c r="B86" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C86" t="s">
-        <v>122</v>
+        <v>418</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
@@ -2511,10 +2811,10 @@
         <v>103</v>
       </c>
       <c r="B87" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C87" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
@@ -2522,10 +2822,10 @@
         <v>103</v>
       </c>
       <c r="B88" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C88" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
@@ -2533,51 +2833,54 @@
         <v>103</v>
       </c>
       <c r="B89" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C89" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>12</v>
+        <v>103</v>
       </c>
       <c r="B90" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C90" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>12</v>
+        <v>103</v>
       </c>
       <c r="B91" t="s">
-        <v>130</v>
+        <v>123</v>
+      </c>
+      <c r="C91" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>12</v>
+        <v>103</v>
       </c>
       <c r="B92" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C92" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>12</v>
+        <v>103</v>
       </c>
       <c r="B93" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C93" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
@@ -2585,10 +2888,10 @@
         <v>12</v>
       </c>
       <c r="B94" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C94" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
@@ -2596,10 +2899,7 @@
         <v>12</v>
       </c>
       <c r="B95" t="s">
-        <v>137</v>
-      </c>
-      <c r="C95" t="s">
-        <v>70</v>
+        <v>130</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
@@ -2607,12 +2907,21 @@
         <v>12</v>
       </c>
       <c r="B96" t="s">
-        <v>138</v>
+        <v>131</v>
+      </c>
+      <c r="C96" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>12</v>
+      </c>
       <c r="B97" t="s">
-        <v>139</v>
+        <v>133</v>
+      </c>
+      <c r="C97" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
@@ -2620,7 +2929,10 @@
         <v>12</v>
       </c>
       <c r="B98" t="s">
-        <v>140</v>
+        <v>135</v>
+      </c>
+      <c r="C98" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
@@ -2628,7 +2940,10 @@
         <v>12</v>
       </c>
       <c r="B99" t="s">
-        <v>141</v>
+        <v>137</v>
+      </c>
+      <c r="C99" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
@@ -2636,12 +2951,12 @@
         <v>12</v>
       </c>
       <c r="B100" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B101" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
@@ -2649,21 +2964,15 @@
         <v>12</v>
       </c>
       <c r="B102" t="s">
-        <v>144</v>
-      </c>
-      <c r="C102" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>146</v>
+        <v>12</v>
       </c>
       <c r="B103" t="s">
-        <v>144</v>
-      </c>
-      <c r="C103" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
@@ -2671,21 +2980,12 @@
         <v>12</v>
       </c>
       <c r="B104" t="s">
-        <v>147</v>
-      </c>
-      <c r="C104" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A105" t="s">
-        <v>146</v>
-      </c>
       <c r="B105" t="s">
-        <v>147</v>
-      </c>
-      <c r="C105" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
@@ -2693,10 +2993,10 @@
         <v>12</v>
       </c>
       <c r="B106" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C106" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
@@ -2704,10 +3004,10 @@
         <v>146</v>
       </c>
       <c r="B107" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C107" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
@@ -2715,10 +3015,10 @@
         <v>12</v>
       </c>
       <c r="B108" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C108" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
@@ -2726,10 +3026,10 @@
         <v>146</v>
       </c>
       <c r="B109" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C109" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
@@ -2737,21 +3037,21 @@
         <v>12</v>
       </c>
       <c r="B110" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C110" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>12</v>
+        <v>146</v>
       </c>
       <c r="B111" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C111" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
@@ -2759,28 +3059,43 @@
         <v>12</v>
       </c>
       <c r="B112" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C112" t="s">
-        <v>11</v>
+        <v>152</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
+        <v>146</v>
+      </c>
+      <c r="B113" t="s">
+        <v>151</v>
+      </c>
+      <c r="C113" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
         <v>12</v>
       </c>
-      <c r="B113" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B114" t="s">
-        <v>159</v>
+        <v>153</v>
+      </c>
+      <c r="C114" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>12</v>
+      </c>
       <c r="B115" t="s">
-        <v>160</v>
+        <v>155</v>
+      </c>
+      <c r="C115" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
@@ -2788,7 +3103,10 @@
         <v>12</v>
       </c>
       <c r="B116" t="s">
-        <v>161</v>
+        <v>157</v>
+      </c>
+      <c r="C116" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
@@ -2796,42 +3114,42 @@
         <v>12</v>
       </c>
       <c r="B117" t="s">
-        <v>162</v>
-      </c>
-      <c r="C117" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>164</v>
+        <v>12</v>
       </c>
       <c r="B118" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>164</v>
+        <v>12</v>
       </c>
       <c r="B119" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>164</v>
+        <v>12</v>
       </c>
       <c r="B120" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>164</v>
+        <v>12</v>
       </c>
       <c r="B121" t="s">
-        <v>168</v>
+        <v>162</v>
+      </c>
+      <c r="C121" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
@@ -2839,7 +3157,10 @@
         <v>164</v>
       </c>
       <c r="B122" t="s">
-        <v>169</v>
+        <v>165</v>
+      </c>
+      <c r="C122" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
@@ -2847,7 +3168,10 @@
         <v>164</v>
       </c>
       <c r="B123" t="s">
-        <v>170</v>
+        <v>166</v>
+      </c>
+      <c r="C123" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
@@ -2855,7 +3179,10 @@
         <v>164</v>
       </c>
       <c r="B124" t="s">
-        <v>171</v>
+        <v>167</v>
+      </c>
+      <c r="C124" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
@@ -2863,7 +3190,10 @@
         <v>164</v>
       </c>
       <c r="B125" t="s">
-        <v>172</v>
+        <v>168</v>
+      </c>
+      <c r="C125" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
@@ -2871,7 +3201,10 @@
         <v>164</v>
       </c>
       <c r="B126" t="s">
-        <v>173</v>
+        <v>169</v>
+      </c>
+      <c r="C126" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
@@ -2879,7 +3212,10 @@
         <v>164</v>
       </c>
       <c r="B127" t="s">
-        <v>174</v>
+        <v>170</v>
+      </c>
+      <c r="C127" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
@@ -2887,7 +3223,10 @@
         <v>164</v>
       </c>
       <c r="B128" t="s">
-        <v>175</v>
+        <v>171</v>
+      </c>
+      <c r="C128" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
@@ -2895,7 +3234,10 @@
         <v>164</v>
       </c>
       <c r="B129" t="s">
-        <v>176</v>
+        <v>172</v>
+      </c>
+      <c r="C129" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
@@ -2903,7 +3245,10 @@
         <v>164</v>
       </c>
       <c r="B130" t="s">
-        <v>177</v>
+        <v>173</v>
+      </c>
+      <c r="C130" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
@@ -2911,7 +3256,10 @@
         <v>164</v>
       </c>
       <c r="B131" t="s">
-        <v>178</v>
+        <v>174</v>
+      </c>
+      <c r="C131" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
@@ -2919,10 +3267,10 @@
         <v>164</v>
       </c>
       <c r="B132" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C132" t="s">
-        <v>180</v>
+        <v>435</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
@@ -2930,10 +3278,10 @@
         <v>164</v>
       </c>
       <c r="B133" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C133" t="s">
-        <v>182</v>
+        <v>426</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
@@ -2941,7 +3289,10 @@
         <v>164</v>
       </c>
       <c r="B134" t="s">
-        <v>183</v>
+        <v>177</v>
+      </c>
+      <c r="C134" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
@@ -2949,7 +3300,10 @@
         <v>164</v>
       </c>
       <c r="B135" t="s">
-        <v>184</v>
+        <v>178</v>
+      </c>
+      <c r="C135" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
@@ -2957,7 +3311,10 @@
         <v>164</v>
       </c>
       <c r="B136" t="s">
-        <v>185</v>
+        <v>179</v>
+      </c>
+      <c r="C136" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
@@ -2965,7 +3322,10 @@
         <v>164</v>
       </c>
       <c r="B137" t="s">
-        <v>186</v>
+        <v>181</v>
+      </c>
+      <c r="C137" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
@@ -2973,7 +3333,10 @@
         <v>164</v>
       </c>
       <c r="B138" t="s">
-        <v>187</v>
+        <v>183</v>
+      </c>
+      <c r="C138" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
@@ -2981,7 +3344,10 @@
         <v>164</v>
       </c>
       <c r="B139" t="s">
-        <v>188</v>
+        <v>184</v>
+      </c>
+      <c r="C139" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
@@ -2989,7 +3355,10 @@
         <v>164</v>
       </c>
       <c r="B140" t="s">
-        <v>189</v>
+        <v>185</v>
+      </c>
+      <c r="C140" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
@@ -2997,7 +3366,10 @@
         <v>164</v>
       </c>
       <c r="B141" t="s">
-        <v>190</v>
+        <v>186</v>
+      </c>
+      <c r="C141" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
@@ -3005,51 +3377,54 @@
         <v>164</v>
       </c>
       <c r="B142" t="s">
-        <v>191</v>
+        <v>187</v>
+      </c>
+      <c r="C142" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="B143" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C143" t="s">
-        <v>193</v>
+        <v>438</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="B144" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C144" t="s">
-        <v>195</v>
+        <v>439</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="B145" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C145" t="s">
-        <v>197</v>
+        <v>440</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="B146" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C146" t="s">
-        <v>199</v>
+        <v>441</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
@@ -3057,64 +3432,76 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C147" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>202</v>
+        <v>146</v>
       </c>
       <c r="B148" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="C148" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>205</v>
+        <v>146</v>
       </c>
       <c r="B149" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C149" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>202</v>
+        <v>146</v>
       </c>
       <c r="B150" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="C150" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
+        <v>146</v>
+      </c>
+      <c r="B151" t="s">
+        <v>200</v>
+      </c>
+      <c r="C151" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>202</v>
+      </c>
+      <c r="B152" t="s">
+        <v>203</v>
+      </c>
+      <c r="C152" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
         <v>205</v>
       </c>
-      <c r="B151" t="s">
-        <v>206</v>
-      </c>
-      <c r="C151" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B152" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B153" t="s">
-        <v>209</v>
+        <v>203</v>
+      </c>
+      <c r="C153" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
@@ -3122,10 +3509,10 @@
         <v>202</v>
       </c>
       <c r="B154" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C154" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
@@ -3133,207 +3520,228 @@
         <v>205</v>
       </c>
       <c r="B155" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C155" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A156" t="s">
-        <v>212</v>
-      </c>
       <c r="B156" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C156" t="s">
-        <v>399</v>
+        <v>479</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A157" t="s">
-        <v>214</v>
-      </c>
       <c r="B157" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C157" t="s">
-        <v>399</v>
+        <v>480</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="B158" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C158" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="B159" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="C159" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="B160" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C160" t="s">
-        <v>220</v>
+        <v>399</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B161" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="C161" t="s">
-        <v>51</v>
+        <v>399</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="B162" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="C162" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="B163" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C163" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B164" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="C164" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B165" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="C165" t="s">
-        <v>229</v>
+        <v>51</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B166" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="C166" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A167" t="s">
+        <v>224</v>
+      </c>
       <c r="B167" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="C167" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
+        <v>226</v>
+      </c>
       <c r="B168" t="s">
-        <v>234</v>
+        <v>226</v>
+      </c>
+      <c r="C168" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
+        <v>228</v>
+      </c>
       <c r="B169" t="s">
-        <v>235</v>
+        <v>228</v>
+      </c>
+      <c r="C169" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B170" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C170" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B171" t="s">
-        <v>239</v>
+        <v>233</v>
+      </c>
+      <c r="C171" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B172" t="s">
-        <v>240</v>
+        <v>234</v>
+      </c>
+      <c r="C172" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B173" t="s">
-        <v>241</v>
+        <v>235</v>
+      </c>
+      <c r="C173" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B174" t="s">
-        <v>243</v>
+        <v>237</v>
+      </c>
+      <c r="C174" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A175" t="s">
-        <v>242</v>
-      </c>
       <c r="B175" t="s">
-        <v>244</v>
+        <v>239</v>
+      </c>
+      <c r="C175" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A176" t="s">
-        <v>242</v>
-      </c>
       <c r="B176" t="s">
-        <v>245</v>
+        <v>240</v>
+      </c>
+      <c r="C176" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A177" t="s">
-        <v>242</v>
-      </c>
       <c r="B177" t="s">
-        <v>246</v>
+        <v>241</v>
+      </c>
+      <c r="C177" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.35">
@@ -3341,136 +3749,148 @@
         <v>242</v>
       </c>
       <c r="B178" t="s">
-        <v>247</v>
+        <v>243</v>
+      </c>
+      <c r="C178" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A179" t="s">
+        <v>242</v>
+      </c>
       <c r="B179" t="s">
-        <v>248</v>
+        <v>244</v>
+      </c>
+      <c r="C179" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A180" t="s">
+        <v>242</v>
+      </c>
       <c r="B180" t="s">
-        <v>249</v>
+        <v>245</v>
+      </c>
+      <c r="C180" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B181" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C181" t="s">
-        <v>389</v>
+        <v>447</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A182" t="s">
+        <v>242</v>
+      </c>
       <c r="B182" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="C182" t="s">
-        <v>253</v>
+        <v>448</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B183" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C183" t="s">
-        <v>390</v>
+        <v>449</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B184" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C184" t="s">
-        <v>256</v>
+        <v>450</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A185" t="s">
+        <v>250</v>
+      </c>
       <c r="B185" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="C185" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B186" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="C186" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B187" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="C187" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B188" t="s">
+        <v>255</v>
+      </c>
+      <c r="C188" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B189" t="s">
+        <v>257</v>
+      </c>
+      <c r="C189" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B190" t="s">
+        <v>258</v>
+      </c>
+      <c r="C190" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B191" t="s">
+        <v>260</v>
+      </c>
+      <c r="C191" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B192" t="s">
         <v>261</v>
       </c>
-      <c r="C188" t="s">
+      <c r="C192" t="s">
         <v>259</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A189" t="s">
-        <v>262</v>
-      </c>
-      <c r="B189" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A190" t="s">
-        <v>36</v>
-      </c>
-      <c r="B190" t="s">
-        <v>264</v>
-      </c>
-      <c r="C190" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A191" t="s">
-        <v>36</v>
-      </c>
-      <c r="B191" t="s">
-        <v>265</v>
-      </c>
-      <c r="C191" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A192" t="s">
-        <v>36</v>
-      </c>
-      <c r="B192" t="s">
-        <v>267</v>
-      </c>
-      <c r="C192" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>36</v>
+        <v>262</v>
       </c>
       <c r="B193" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C193" t="s">
-        <v>400</v>
+        <v>451</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.35">
@@ -3478,10 +3898,10 @@
         <v>36</v>
       </c>
       <c r="B194" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C194" t="s">
-        <v>270</v>
+        <v>94</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.35">
@@ -3489,10 +3909,10 @@
         <v>36</v>
       </c>
       <c r="B195" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="C195" t="s">
-        <v>216</v>
+        <v>266</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.35">
@@ -3500,10 +3920,10 @@
         <v>36</v>
       </c>
       <c r="B196" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C196" t="s">
-        <v>63</v>
+        <v>223</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.35">
@@ -3511,10 +3931,10 @@
         <v>36</v>
       </c>
       <c r="B197" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C197" t="s">
-        <v>274</v>
+        <v>400</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.35">
@@ -3522,10 +3942,10 @@
         <v>36</v>
       </c>
       <c r="B198" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C198" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.35">
@@ -3533,10 +3953,10 @@
         <v>36</v>
       </c>
       <c r="B199" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="C199" t="s">
-        <v>278</v>
+        <v>216</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.35">
@@ -3544,10 +3964,10 @@
         <v>36</v>
       </c>
       <c r="B200" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="C200" t="s">
-        <v>280</v>
+        <v>63</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.35">
@@ -3555,10 +3975,10 @@
         <v>36</v>
       </c>
       <c r="B201" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="C201" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.35">
@@ -3566,10 +3986,10 @@
         <v>36</v>
       </c>
       <c r="B202" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="C202" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.35">
@@ -3577,10 +3997,10 @@
         <v>36</v>
       </c>
       <c r="B203" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="C203" t="s">
-        <v>366</v>
+        <v>278</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.35">
@@ -3588,10 +4008,10 @@
         <v>36</v>
       </c>
       <c r="B204" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="C204" t="s">
-        <v>180</v>
+        <v>280</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.35">
@@ -3599,10 +4019,10 @@
         <v>36</v>
       </c>
       <c r="B205" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="C205" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.35">
@@ -3610,10 +4030,10 @@
         <v>36</v>
       </c>
       <c r="B206" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="C206" t="s">
-        <v>182</v>
+        <v>284</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.35">
@@ -3621,10 +4041,10 @@
         <v>36</v>
       </c>
       <c r="B207" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="C207" t="s">
-        <v>291</v>
+        <v>366</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.35">
@@ -3632,10 +4052,10 @@
         <v>36</v>
       </c>
       <c r="B208" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="C208" t="s">
-        <v>394</v>
+        <v>180</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.35">
@@ -3643,10 +4063,10 @@
         <v>36</v>
       </c>
       <c r="B209" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="C209" t="s">
-        <v>395</v>
+        <v>288</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.35">
@@ -3654,10 +4074,10 @@
         <v>36</v>
       </c>
       <c r="B210" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C210" t="s">
-        <v>396</v>
+        <v>182</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.35">
@@ -3665,10 +4085,10 @@
         <v>36</v>
       </c>
       <c r="B211" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C211" t="s">
-        <v>38</v>
+        <v>291</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.35">
@@ -3676,7 +4096,10 @@
         <v>36</v>
       </c>
       <c r="B212" t="s">
-        <v>296</v>
+        <v>292</v>
+      </c>
+      <c r="C212" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.35">
@@ -3684,7 +4107,10 @@
         <v>36</v>
       </c>
       <c r="B213" t="s">
-        <v>297</v>
+        <v>293</v>
+      </c>
+      <c r="C213" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.35">
@@ -3692,7 +4118,10 @@
         <v>36</v>
       </c>
       <c r="B214" t="s">
-        <v>298</v>
+        <v>294</v>
+      </c>
+      <c r="C214" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.35">
@@ -3700,10 +4129,10 @@
         <v>36</v>
       </c>
       <c r="B215" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C215" t="s">
-        <v>392</v>
+        <v>38</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.35">
@@ -3711,10 +4140,10 @@
         <v>36</v>
       </c>
       <c r="B216" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C216" t="s">
-        <v>301</v>
+        <v>452</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.35">
@@ -3722,10 +4151,10 @@
         <v>36</v>
       </c>
       <c r="B217" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="C217" t="s">
-        <v>303</v>
+        <v>483</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.35">
@@ -3733,10 +4162,10 @@
         <v>36</v>
       </c>
       <c r="B218" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="C218" t="s">
-        <v>393</v>
+        <v>484</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.35">
@@ -3744,10 +4173,10 @@
         <v>36</v>
       </c>
       <c r="B219" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="C219" t="s">
-        <v>306</v>
+        <v>392</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.35">
@@ -3755,40 +4184,76 @@
         <v>36</v>
       </c>
       <c r="B220" t="s">
+        <v>300</v>
+      </c>
+      <c r="C220" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A221" t="s">
+        <v>36</v>
+      </c>
+      <c r="B221" t="s">
+        <v>302</v>
+      </c>
+      <c r="C221" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A222" t="s">
+        <v>36</v>
+      </c>
+      <c r="B222" t="s">
+        <v>304</v>
+      </c>
+      <c r="C222" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A223" t="s">
+        <v>36</v>
+      </c>
+      <c r="B223" t="s">
+        <v>305</v>
+      </c>
+      <c r="C223" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A224" t="s">
+        <v>36</v>
+      </c>
+      <c r="B224" t="s">
         <v>307</v>
       </c>
-      <c r="C220" t="s">
+      <c r="C224" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B221" t="s">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A225" t="s">
+        <v>36</v>
+      </c>
+      <c r="B225" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B222" t="s">
+      <c r="C225" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A226" t="s">
+        <v>36</v>
+      </c>
+      <c r="B226" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B223" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B224" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B225" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B226" t="s">
-        <v>314</v>
+      <c r="C226" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.35">
@@ -3796,10 +4261,10 @@
         <v>36</v>
       </c>
       <c r="B227" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C227" t="s">
-        <v>401</v>
+        <v>455</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.35">
@@ -3807,10 +4272,10 @@
         <v>36</v>
       </c>
       <c r="B228" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C228" t="s">
-        <v>402</v>
+        <v>456</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.35">
@@ -3818,10 +4283,10 @@
         <v>36</v>
       </c>
       <c r="B229" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C229" t="s">
-        <v>403</v>
+        <v>457</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.35">
@@ -3829,7 +4294,10 @@
         <v>36</v>
       </c>
       <c r="B230" t="s">
-        <v>318</v>
+        <v>314</v>
+      </c>
+      <c r="C230" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.35">
@@ -3837,7 +4305,10 @@
         <v>36</v>
       </c>
       <c r="B231" t="s">
-        <v>319</v>
+        <v>315</v>
+      </c>
+      <c r="C231" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.35">
@@ -3845,7 +4316,10 @@
         <v>36</v>
       </c>
       <c r="B232" t="s">
-        <v>320</v>
+        <v>316</v>
+      </c>
+      <c r="C232" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.35">
@@ -3853,7 +4327,10 @@
         <v>36</v>
       </c>
       <c r="B233" t="s">
-        <v>321</v>
+        <v>317</v>
+      </c>
+      <c r="C233" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.35">
@@ -3861,7 +4338,10 @@
         <v>36</v>
       </c>
       <c r="B234" t="s">
-        <v>322</v>
+        <v>318</v>
+      </c>
+      <c r="C234" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.35">
@@ -3869,7 +4349,10 @@
         <v>36</v>
       </c>
       <c r="B235" t="s">
-        <v>323</v>
+        <v>319</v>
+      </c>
+      <c r="C235" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.35">
@@ -3877,7 +4360,10 @@
         <v>36</v>
       </c>
       <c r="B236" t="s">
-        <v>324</v>
+        <v>320</v>
+      </c>
+      <c r="C236" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.35">
@@ -3885,7 +4371,10 @@
         <v>36</v>
       </c>
       <c r="B237" t="s">
-        <v>325</v>
+        <v>321</v>
+      </c>
+      <c r="C237" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.35">
@@ -3893,130 +4382,142 @@
         <v>36</v>
       </c>
       <c r="B238" t="s">
-        <v>326</v>
+        <v>322</v>
+      </c>
+      <c r="C238" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>327</v>
+        <v>36</v>
       </c>
       <c r="B239" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="C239" t="s">
-        <v>180</v>
+        <v>464</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>327</v>
+        <v>36</v>
       </c>
       <c r="B240" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="C240" t="s">
-        <v>288</v>
+        <v>465</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>327</v>
+        <v>36</v>
       </c>
       <c r="B241" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="C241" t="s">
-        <v>331</v>
+        <v>466</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>327</v>
+        <v>36</v>
       </c>
       <c r="B242" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="C242" t="s">
-        <v>333</v>
+        <v>467</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>236</v>
+        <v>327</v>
       </c>
       <c r="B243" t="s">
-        <v>232</v>
+        <v>328</v>
       </c>
       <c r="C243" t="s">
-        <v>232</v>
+        <v>180</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>236</v>
+        <v>327</v>
       </c>
       <c r="B244" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C244" t="s">
-        <v>335</v>
+        <v>288</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>236</v>
+        <v>327</v>
       </c>
       <c r="B245" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="C245" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>236</v>
+        <v>327</v>
       </c>
       <c r="B246" t="s">
-        <v>238</v>
+        <v>332</v>
       </c>
       <c r="C246" t="s">
-        <v>238</v>
+        <v>333</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>236</v>
+        <v>327</v>
       </c>
       <c r="B247" t="s">
-        <v>338</v>
+        <v>406</v>
+      </c>
+      <c r="C247" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>236</v>
+        <v>327</v>
       </c>
       <c r="B248" t="s">
-        <v>339</v>
+        <v>407</v>
+      </c>
+      <c r="C248" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>236</v>
+        <v>327</v>
       </c>
       <c r="B249" t="s">
-        <v>340</v>
+        <v>408</v>
+      </c>
+      <c r="C249" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>236</v>
+        <v>327</v>
       </c>
       <c r="B250" t="s">
-        <v>341</v>
+        <v>409</v>
       </c>
       <c r="C250" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.35">
@@ -4024,10 +4525,10 @@
         <v>236</v>
       </c>
       <c r="B251" t="s">
-        <v>343</v>
+        <v>232</v>
       </c>
       <c r="C251" t="s">
-        <v>344</v>
+        <v>232</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.35">
@@ -4035,7 +4536,10 @@
         <v>236</v>
       </c>
       <c r="B252" t="s">
-        <v>345</v>
+        <v>334</v>
+      </c>
+      <c r="C252" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.35">
@@ -4043,7 +4547,10 @@
         <v>236</v>
       </c>
       <c r="B253" t="s">
-        <v>346</v>
+        <v>336</v>
+      </c>
+      <c r="C253" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.35">
@@ -4051,7 +4558,10 @@
         <v>236</v>
       </c>
       <c r="B254" t="s">
-        <v>347</v>
+        <v>238</v>
+      </c>
+      <c r="C254" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.35">
@@ -4059,10 +4569,10 @@
         <v>236</v>
       </c>
       <c r="B255" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="C255" t="s">
-        <v>11</v>
+        <v>468</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.35">
@@ -4070,10 +4580,10 @@
         <v>236</v>
       </c>
       <c r="B256" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="C256" t="s">
-        <v>350</v>
+        <v>485</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.35">
@@ -4081,10 +4591,10 @@
         <v>236</v>
       </c>
       <c r="B257" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
       <c r="C257" t="s">
-        <v>352</v>
+        <v>486</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.35">
@@ -4092,7 +4602,10 @@
         <v>236</v>
       </c>
       <c r="B258" t="s">
-        <v>353</v>
+        <v>341</v>
+      </c>
+      <c r="C258" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.35">
@@ -4100,114 +4613,117 @@
         <v>236</v>
       </c>
       <c r="B259" t="s">
-        <v>354</v>
+        <v>343</v>
+      </c>
+      <c r="C259" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
-        <v>355</v>
+        <v>236</v>
       </c>
       <c r="B260" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
       <c r="C260" t="s">
-        <v>223</v>
+        <v>469</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
-        <v>355</v>
+        <v>236</v>
       </c>
       <c r="B261" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
       <c r="C261" t="s">
-        <v>366</v>
+        <v>346</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
-        <v>355</v>
+        <v>236</v>
       </c>
       <c r="B262" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
       <c r="C262" t="s">
-        <v>63</v>
+        <v>470</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
-        <v>355</v>
+        <v>236</v>
       </c>
       <c r="B263" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="C263" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
-        <v>355</v>
+        <v>236</v>
       </c>
       <c r="B264" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
       <c r="C264" t="s">
-        <v>51</v>
+        <v>350</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
-        <v>355</v>
+        <v>236</v>
       </c>
       <c r="B265" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="C265" t="s">
-        <v>180</v>
+        <v>352</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
-        <v>355</v>
+        <v>236</v>
       </c>
       <c r="B266" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="C266" t="s">
-        <v>333</v>
+        <v>471</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
-        <v>355</v>
+        <v>236</v>
       </c>
       <c r="B267" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="C267" t="s">
-        <v>331</v>
+        <v>487</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="B268" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="C268" t="s">
-        <v>405</v>
+        <v>223</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="B269" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C269" t="s">
         <v>366</v>
@@ -4215,159 +4731,298 @@
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="B270" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="C270" t="s">
-        <v>366</v>
+        <v>63</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="B271" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="C271" t="s">
-        <v>404</v>
+        <v>55</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="B272" t="s">
-        <v>369</v>
+        <v>360</v>
+      </c>
+      <c r="C272" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
-        <v>370</v>
+        <v>355</v>
       </c>
       <c r="B273" t="s">
-        <v>371</v>
+        <v>361</v>
+      </c>
+      <c r="C273" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A274" t="s">
+        <v>355</v>
+      </c>
       <c r="B274" t="s">
-        <v>372</v>
+        <v>362</v>
+      </c>
+      <c r="C274" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A275" t="s">
+        <v>355</v>
+      </c>
       <c r="B275" t="s">
-        <v>373</v>
+        <v>363</v>
+      </c>
+      <c r="C275" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A276" t="s">
+        <v>364</v>
+      </c>
       <c r="B276" t="s">
-        <v>374</v>
+        <v>365</v>
+      </c>
+      <c r="C276" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A277" t="s">
+        <v>364</v>
+      </c>
       <c r="B277" t="s">
-        <v>375</v>
+        <v>366</v>
+      </c>
+      <c r="C277" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A278" t="s">
+        <v>364</v>
+      </c>
       <c r="B278" t="s">
-        <v>376</v>
+        <v>367</v>
+      </c>
+      <c r="C278" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A279" t="s">
+        <v>364</v>
+      </c>
       <c r="B279" t="s">
-        <v>377</v>
+        <v>368</v>
+      </c>
+      <c r="C279" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A280" t="s">
+        <v>364</v>
+      </c>
       <c r="B280" t="s">
-        <v>378</v>
+        <v>369</v>
+      </c>
+      <c r="C280" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="B281" t="s">
-        <v>380</v>
+        <v>371</v>
+      </c>
+      <c r="C281" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
       <c r="B282" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="C282" t="s">
-        <v>223</v>
+        <v>473</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
       <c r="B283" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="C283" t="s">
-        <v>55</v>
+        <v>373</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
       <c r="B284" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="C284" t="s">
-        <v>51</v>
+        <v>474</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
       <c r="B285" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="C285" t="s">
-        <v>63</v>
+        <v>375</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
       <c r="B286" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="C286" t="s">
-        <v>288</v>
+        <v>475</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
       <c r="B287" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="C287" t="s">
-        <v>180</v>
+        <v>377</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
+        <v>370</v>
+      </c>
+      <c r="B288" t="s">
+        <v>378</v>
+      </c>
+      <c r="C288" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A289" t="s">
+        <v>379</v>
+      </c>
+      <c r="B289" t="s">
+        <v>380</v>
+      </c>
+      <c r="C289" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A290" t="s">
+        <v>381</v>
+      </c>
+      <c r="B290" t="s">
+        <v>382</v>
+      </c>
+      <c r="C290" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A291" t="s">
+        <v>381</v>
+      </c>
+      <c r="B291" t="s">
+        <v>383</v>
+      </c>
+      <c r="C291" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A292" t="s">
+        <v>381</v>
+      </c>
+      <c r="B292" t="s">
+        <v>384</v>
+      </c>
+      <c r="C292" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A293" t="s">
+        <v>381</v>
+      </c>
+      <c r="B293" t="s">
+        <v>385</v>
+      </c>
+      <c r="C293" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A294" t="s">
+        <v>381</v>
+      </c>
+      <c r="B294" t="s">
+        <v>386</v>
+      </c>
+      <c r="C294" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A295" t="s">
+        <v>381</v>
+      </c>
+      <c r="B295" t="s">
+        <v>387</v>
+      </c>
+      <c r="C295" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A296" t="s">
         <v>388</v>
       </c>
-      <c r="B288" t="s">
+      <c r="B296" t="s">
         <v>388</v>
       </c>
-      <c r="C288" t="s">
+      <c r="C296" t="s">
         <v>216</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update naming conventions as aligned from meeting with @sbreitbart-NOAA and @kellijohnson-NOAA
</commit_message>
<xml_diff>
--- a/inst/resources/bam_var_names.xlsx
+++ b/inst/resources/bam_var_names.xlsx
@@ -417,9 +417,6 @@
     <t>log_R0</t>
   </si>
   <si>
-    <t>ln_R0</t>
-  </si>
-  <si>
     <t>steep</t>
   </si>
   <si>
@@ -1212,9 +1209,6 @@
     <t>indices_cv</t>
   </si>
   <si>
-    <t>virgin_recruitment</t>
-  </si>
-  <si>
     <t>recruitment_lag</t>
   </si>
   <si>
@@ -1507,6 +1501,12 @@
   </si>
   <si>
     <t>f_prop_d</t>
+  </si>
+  <si>
+    <t>log_recruitment_unfished</t>
+  </si>
+  <si>
+    <t>recruitment_unfished_bc</t>
   </si>
 </sst>
 </file>
@@ -1861,8 +1861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C296"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2025,7 +2025,7 @@
         <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -2036,7 +2036,7 @@
         <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -2154,7 +2154,7 @@
         <v>39</v>
       </c>
       <c r="C27" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -2165,7 +2165,7 @@
         <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -2173,10 +2173,10 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C29" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -2316,10 +2316,10 @@
         <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C42" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
@@ -2338,10 +2338,10 @@
         <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C44" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
@@ -2360,10 +2360,10 @@
         <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C46" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
@@ -2396,7 +2396,7 @@
         <v>66</v>
       </c>
       <c r="C49" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -2407,7 +2407,7 @@
         <v>67</v>
       </c>
       <c r="C50" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
@@ -2418,7 +2418,7 @@
         <v>68</v>
       </c>
       <c r="C51" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -2451,7 +2451,7 @@
         <v>72</v>
       </c>
       <c r="C54" t="s">
-        <v>397</v>
+        <v>495</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
@@ -2462,7 +2462,7 @@
         <v>73</v>
       </c>
       <c r="C55" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
@@ -2792,7 +2792,7 @@
         <v>116</v>
       </c>
       <c r="C85" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
@@ -2803,7 +2803,7 @@
         <v>117</v>
       </c>
       <c r="C86" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
@@ -2910,7 +2910,7 @@
         <v>131</v>
       </c>
       <c r="C96" t="s">
-        <v>132</v>
+        <v>494</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
@@ -2918,10 +2918,10 @@
         <v>12</v>
       </c>
       <c r="B97" t="s">
+        <v>132</v>
+      </c>
+      <c r="C97" t="s">
         <v>133</v>
-      </c>
-      <c r="C97" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
@@ -2929,10 +2929,10 @@
         <v>12</v>
       </c>
       <c r="B98" t="s">
+        <v>134</v>
+      </c>
+      <c r="C98" t="s">
         <v>135</v>
-      </c>
-      <c r="C98" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
@@ -2940,7 +2940,7 @@
         <v>12</v>
       </c>
       <c r="B99" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C99" t="s">
         <v>70</v>
@@ -2951,12 +2951,12 @@
         <v>12</v>
       </c>
       <c r="B100" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B101" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
@@ -2964,7 +2964,7 @@
         <v>12</v>
       </c>
       <c r="B102" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
@@ -2972,7 +2972,7 @@
         <v>12</v>
       </c>
       <c r="B103" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
@@ -2980,12 +2980,12 @@
         <v>12</v>
       </c>
       <c r="B104" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B105" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
@@ -2993,21 +2993,21 @@
         <v>12</v>
       </c>
       <c r="B106" t="s">
+        <v>143</v>
+      </c>
+      <c r="C106" t="s">
         <v>144</v>
-      </c>
-      <c r="C106" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B107" t="s">
+        <v>143</v>
+      </c>
+      <c r="C107" t="s">
         <v>144</v>
-      </c>
-      <c r="C107" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
@@ -3015,21 +3015,21 @@
         <v>12</v>
       </c>
       <c r="B108" t="s">
+        <v>146</v>
+      </c>
+      <c r="C108" t="s">
         <v>147</v>
-      </c>
-      <c r="C108" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
+        <v>145</v>
+      </c>
+      <c r="B109" t="s">
         <v>146</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C109" t="s">
         <v>147</v>
-      </c>
-      <c r="C109" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
@@ -3037,21 +3037,21 @@
         <v>12</v>
       </c>
       <c r="B110" t="s">
+        <v>148</v>
+      </c>
+      <c r="C110" t="s">
         <v>149</v>
-      </c>
-      <c r="C110" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B111" t="s">
+        <v>148</v>
+      </c>
+      <c r="C111" t="s">
         <v>149</v>
-      </c>
-      <c r="C111" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
@@ -3059,21 +3059,21 @@
         <v>12</v>
       </c>
       <c r="B112" t="s">
+        <v>150</v>
+      </c>
+      <c r="C112" t="s">
         <v>151</v>
-      </c>
-      <c r="C112" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B113" t="s">
+        <v>150</v>
+      </c>
+      <c r="C113" t="s">
         <v>151</v>
-      </c>
-      <c r="C113" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
@@ -3081,10 +3081,10 @@
         <v>12</v>
       </c>
       <c r="B114" t="s">
+        <v>152</v>
+      </c>
+      <c r="C114" t="s">
         <v>153</v>
-      </c>
-      <c r="C114" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
@@ -3092,10 +3092,10 @@
         <v>12</v>
       </c>
       <c r="B115" t="s">
+        <v>154</v>
+      </c>
+      <c r="C115" t="s">
         <v>155</v>
-      </c>
-      <c r="C115" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
@@ -3103,7 +3103,7 @@
         <v>12</v>
       </c>
       <c r="B116" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C116" t="s">
         <v>11</v>
@@ -3114,7 +3114,7 @@
         <v>12</v>
       </c>
       <c r="B117" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
@@ -3122,7 +3122,7 @@
         <v>12</v>
       </c>
       <c r="B118" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
@@ -3130,7 +3130,7 @@
         <v>12</v>
       </c>
       <c r="B119" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
@@ -3138,7 +3138,7 @@
         <v>12</v>
       </c>
       <c r="B120" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
@@ -3146,485 +3146,485 @@
         <v>12</v>
       </c>
       <c r="B121" t="s">
+        <v>161</v>
+      </c>
+      <c r="C121" t="s">
         <v>162</v>
-      </c>
-      <c r="C121" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
+        <v>163</v>
+      </c>
+      <c r="B122" t="s">
         <v>164</v>
       </c>
-      <c r="B122" t="s">
-        <v>165</v>
-      </c>
       <c r="C122" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B123" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C123" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B124" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C124" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B125" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C125" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B126" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C126" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B127" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C127" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B128" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C128" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B129" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C129" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B130" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C130" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B131" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C131" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B132" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C132" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B133" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C133" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B134" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C134" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B135" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C135" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B136" t="s">
+        <v>178</v>
+      </c>
+      <c r="C136" t="s">
         <v>179</v>
-      </c>
-      <c r="C136" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B137" t="s">
+        <v>180</v>
+      </c>
+      <c r="C137" t="s">
         <v>181</v>
-      </c>
-      <c r="C137" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B138" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C138" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B139" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C139" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B140" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C140" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B141" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C141" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B142" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C142" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B143" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C143" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B144" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C144" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B145" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C145" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B146" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C146" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B147" t="s">
+        <v>191</v>
+      </c>
+      <c r="C147" t="s">
         <v>192</v>
-      </c>
-      <c r="C147" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B148" t="s">
+        <v>193</v>
+      </c>
+      <c r="C148" t="s">
         <v>194</v>
-      </c>
-      <c r="C148" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B149" t="s">
+        <v>195</v>
+      </c>
+      <c r="C149" t="s">
         <v>196</v>
-      </c>
-      <c r="C149" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B150" t="s">
+        <v>197</v>
+      </c>
+      <c r="C150" t="s">
         <v>198</v>
-      </c>
-      <c r="C150" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B151" t="s">
+        <v>199</v>
+      </c>
+      <c r="C151" t="s">
         <v>200</v>
-      </c>
-      <c r="C151" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
+        <v>201</v>
+      </c>
+      <c r="B152" t="s">
         <v>202</v>
       </c>
-      <c r="B152" t="s">
+      <c r="C152" t="s">
         <v>203</v>
-      </c>
-      <c r="C152" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B153" t="s">
+        <v>202</v>
+      </c>
+      <c r="C153" t="s">
         <v>203</v>
-      </c>
-      <c r="C153" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B154" t="s">
+        <v>205</v>
+      </c>
+      <c r="C154" t="s">
         <v>206</v>
-      </c>
-      <c r="C154" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
+        <v>204</v>
+      </c>
+      <c r="B155" t="s">
         <v>205</v>
       </c>
-      <c r="B155" t="s">
+      <c r="C155" t="s">
         <v>206</v>
-      </c>
-      <c r="C155" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B156" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C156" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B157" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C157" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B158" t="s">
+        <v>209</v>
+      </c>
+      <c r="C158" t="s">
         <v>210</v>
-      </c>
-      <c r="C158" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B159" t="s">
+        <v>209</v>
+      </c>
+      <c r="C159" t="s">
         <v>210</v>
-      </c>
-      <c r="C159" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
+        <v>211</v>
+      </c>
+      <c r="B160" t="s">
         <v>212</v>
       </c>
-      <c r="B160" t="s">
-        <v>213</v>
-      </c>
       <c r="C160" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B161" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C161" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
+        <v>214</v>
+      </c>
+      <c r="B162" t="s">
+        <v>214</v>
+      </c>
+      <c r="C162" t="s">
         <v>215</v>
-      </c>
-      <c r="B162" t="s">
-        <v>215</v>
-      </c>
-      <c r="C162" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
+        <v>216</v>
+      </c>
+      <c r="B163" t="s">
+        <v>216</v>
+      </c>
+      <c r="C163" t="s">
         <v>217</v>
-      </c>
-      <c r="B163" t="s">
-        <v>217</v>
-      </c>
-      <c r="C163" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
+        <v>218</v>
+      </c>
+      <c r="B164" t="s">
+        <v>218</v>
+      </c>
+      <c r="C164" t="s">
         <v>219</v>
-      </c>
-      <c r="B164" t="s">
-        <v>219</v>
-      </c>
-      <c r="C164" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B165" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C165" t="s">
         <v>51</v>
@@ -3632,265 +3632,265 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
+        <v>221</v>
+      </c>
+      <c r="B166" t="s">
+        <v>221</v>
+      </c>
+      <c r="C166" t="s">
         <v>222</v>
-      </c>
-      <c r="B166" t="s">
-        <v>222</v>
-      </c>
-      <c r="C166" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
+        <v>223</v>
+      </c>
+      <c r="B167" t="s">
+        <v>223</v>
+      </c>
+      <c r="C167" t="s">
         <v>224</v>
-      </c>
-      <c r="B167" t="s">
-        <v>224</v>
-      </c>
-      <c r="C167" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
+        <v>225</v>
+      </c>
+      <c r="B168" t="s">
+        <v>225</v>
+      </c>
+      <c r="C168" t="s">
         <v>226</v>
-      </c>
-      <c r="B168" t="s">
-        <v>226</v>
-      </c>
-      <c r="C168" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
+        <v>227</v>
+      </c>
+      <c r="B169" t="s">
+        <v>227</v>
+      </c>
+      <c r="C169" t="s">
         <v>228</v>
-      </c>
-      <c r="B169" t="s">
-        <v>228</v>
-      </c>
-      <c r="C169" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
+        <v>229</v>
+      </c>
+      <c r="B170" t="s">
         <v>230</v>
       </c>
-      <c r="B170" t="s">
+      <c r="C170" t="s">
         <v>231</v>
-      </c>
-      <c r="C170" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B171" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C171" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B172" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C172" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B173" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C173" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
+        <v>235</v>
+      </c>
+      <c r="B174" t="s">
         <v>236</v>
       </c>
-      <c r="B174" t="s">
+      <c r="C174" t="s">
         <v>237</v>
-      </c>
-      <c r="C174" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B175" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C175" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B176" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C176" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B177" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C177" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
+        <v>241</v>
+      </c>
+      <c r="B178" t="s">
         <v>242</v>
       </c>
-      <c r="B178" t="s">
-        <v>243</v>
-      </c>
       <c r="C178" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B179" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C179" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B180" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C180" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B181" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C181" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B182" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C182" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B183" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C183" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B184" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C184" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
+        <v>249</v>
+      </c>
+      <c r="B185" t="s">
         <v>250</v>
       </c>
-      <c r="B185" t="s">
-        <v>251</v>
-      </c>
       <c r="C185" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B186" t="s">
+        <v>251</v>
+      </c>
+      <c r="C186" t="s">
         <v>252</v>
-      </c>
-      <c r="C186" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B187" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C187" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B188" t="s">
+        <v>254</v>
+      </c>
+      <c r="C188" t="s">
         <v>255</v>
-      </c>
-      <c r="C188" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B189" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C189" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B190" t="s">
+        <v>257</v>
+      </c>
+      <c r="C190" t="s">
         <v>258</v>
-      </c>
-      <c r="C190" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B191" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C191" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B192" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C192" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
+        <v>261</v>
+      </c>
+      <c r="B193" t="s">
         <v>262</v>
       </c>
-      <c r="B193" t="s">
-        <v>263</v>
-      </c>
       <c r="C193" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.35">
@@ -3898,7 +3898,7 @@
         <v>36</v>
       </c>
       <c r="B194" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C194" t="s">
         <v>94</v>
@@ -3909,10 +3909,10 @@
         <v>36</v>
       </c>
       <c r="B195" t="s">
+        <v>264</v>
+      </c>
+      <c r="C195" t="s">
         <v>265</v>
-      </c>
-      <c r="C195" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.35">
@@ -3920,10 +3920,10 @@
         <v>36</v>
       </c>
       <c r="B196" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C196" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.35">
@@ -3931,10 +3931,10 @@
         <v>36</v>
       </c>
       <c r="B197" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C197" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.35">
@@ -3942,10 +3942,10 @@
         <v>36</v>
       </c>
       <c r="B198" t="s">
+        <v>268</v>
+      </c>
+      <c r="C198" t="s">
         <v>269</v>
-      </c>
-      <c r="C198" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.35">
@@ -3953,10 +3953,10 @@
         <v>36</v>
       </c>
       <c r="B199" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C199" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.35">
@@ -3964,7 +3964,7 @@
         <v>36</v>
       </c>
       <c r="B200" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C200" t="s">
         <v>63</v>
@@ -3975,10 +3975,10 @@
         <v>36</v>
       </c>
       <c r="B201" t="s">
+        <v>272</v>
+      </c>
+      <c r="C201" t="s">
         <v>273</v>
-      </c>
-      <c r="C201" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.35">
@@ -3986,10 +3986,10 @@
         <v>36</v>
       </c>
       <c r="B202" t="s">
+        <v>274</v>
+      </c>
+      <c r="C202" t="s">
         <v>275</v>
-      </c>
-      <c r="C202" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.35">
@@ -3997,10 +3997,10 @@
         <v>36</v>
       </c>
       <c r="B203" t="s">
+        <v>276</v>
+      </c>
+      <c r="C203" t="s">
         <v>277</v>
-      </c>
-      <c r="C203" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.35">
@@ -4008,10 +4008,10 @@
         <v>36</v>
       </c>
       <c r="B204" t="s">
+        <v>278</v>
+      </c>
+      <c r="C204" t="s">
         <v>279</v>
-      </c>
-      <c r="C204" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.35">
@@ -4019,10 +4019,10 @@
         <v>36</v>
       </c>
       <c r="B205" t="s">
+        <v>280</v>
+      </c>
+      <c r="C205" t="s">
         <v>281</v>
-      </c>
-      <c r="C205" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.35">
@@ -4030,10 +4030,10 @@
         <v>36</v>
       </c>
       <c r="B206" t="s">
+        <v>282</v>
+      </c>
+      <c r="C206" t="s">
         <v>283</v>
-      </c>
-      <c r="C206" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.35">
@@ -4041,10 +4041,10 @@
         <v>36</v>
       </c>
       <c r="B207" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C207" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.35">
@@ -4052,10 +4052,10 @@
         <v>36</v>
       </c>
       <c r="B208" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C208" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.35">
@@ -4063,10 +4063,10 @@
         <v>36</v>
       </c>
       <c r="B209" t="s">
+        <v>286</v>
+      </c>
+      <c r="C209" t="s">
         <v>287</v>
-      </c>
-      <c r="C209" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.35">
@@ -4074,10 +4074,10 @@
         <v>36</v>
       </c>
       <c r="B210" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C210" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.35">
@@ -4085,10 +4085,10 @@
         <v>36</v>
       </c>
       <c r="B211" t="s">
+        <v>289</v>
+      </c>
+      <c r="C211" t="s">
         <v>290</v>
-      </c>
-      <c r="C211" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.35">
@@ -4096,10 +4096,10 @@
         <v>36</v>
       </c>
       <c r="B212" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C212" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.35">
@@ -4107,10 +4107,10 @@
         <v>36</v>
       </c>
       <c r="B213" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C213" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.35">
@@ -4118,10 +4118,10 @@
         <v>36</v>
       </c>
       <c r="B214" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C214" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.35">
@@ -4129,7 +4129,7 @@
         <v>36</v>
       </c>
       <c r="B215" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C215" t="s">
         <v>38</v>
@@ -4140,10 +4140,10 @@
         <v>36</v>
       </c>
       <c r="B216" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C216" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.35">
@@ -4151,10 +4151,10 @@
         <v>36</v>
       </c>
       <c r="B217" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C217" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.35">
@@ -4162,10 +4162,10 @@
         <v>36</v>
       </c>
       <c r="B218" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C218" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.35">
@@ -4173,10 +4173,10 @@
         <v>36</v>
       </c>
       <c r="B219" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C219" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.35">
@@ -4184,10 +4184,10 @@
         <v>36</v>
       </c>
       <c r="B220" t="s">
+        <v>299</v>
+      </c>
+      <c r="C220" t="s">
         <v>300</v>
-      </c>
-      <c r="C220" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.35">
@@ -4195,10 +4195,10 @@
         <v>36</v>
       </c>
       <c r="B221" t="s">
+        <v>301</v>
+      </c>
+      <c r="C221" t="s">
         <v>302</v>
-      </c>
-      <c r="C221" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.35">
@@ -4206,10 +4206,10 @@
         <v>36</v>
       </c>
       <c r="B222" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C222" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.35">
@@ -4217,10 +4217,10 @@
         <v>36</v>
       </c>
       <c r="B223" t="s">
+        <v>304</v>
+      </c>
+      <c r="C223" t="s">
         <v>305</v>
-      </c>
-      <c r="C223" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.35">
@@ -4228,10 +4228,10 @@
         <v>36</v>
       </c>
       <c r="B224" t="s">
+        <v>306</v>
+      </c>
+      <c r="C224" t="s">
         <v>307</v>
-      </c>
-      <c r="C224" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.35">
@@ -4239,10 +4239,10 @@
         <v>36</v>
       </c>
       <c r="B225" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C225" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.35">
@@ -4250,10 +4250,10 @@
         <v>36</v>
       </c>
       <c r="B226" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C226" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.35">
@@ -4261,10 +4261,10 @@
         <v>36</v>
       </c>
       <c r="B227" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C227" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.35">
@@ -4272,10 +4272,10 @@
         <v>36</v>
       </c>
       <c r="B228" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C228" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.35">
@@ -4283,10 +4283,10 @@
         <v>36</v>
       </c>
       <c r="B229" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C229" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.35">
@@ -4294,10 +4294,10 @@
         <v>36</v>
       </c>
       <c r="B230" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C230" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.35">
@@ -4305,10 +4305,10 @@
         <v>36</v>
       </c>
       <c r="B231" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C231" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.35">
@@ -4316,10 +4316,10 @@
         <v>36</v>
       </c>
       <c r="B232" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C232" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.35">
@@ -4327,10 +4327,10 @@
         <v>36</v>
       </c>
       <c r="B233" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C233" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.35">
@@ -4338,10 +4338,10 @@
         <v>36</v>
       </c>
       <c r="B234" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C234" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.35">
@@ -4349,10 +4349,10 @@
         <v>36</v>
       </c>
       <c r="B235" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C235" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.35">
@@ -4360,10 +4360,10 @@
         <v>36</v>
       </c>
       <c r="B236" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C236" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.35">
@@ -4371,10 +4371,10 @@
         <v>36</v>
       </c>
       <c r="B237" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C237" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.35">
@@ -4382,10 +4382,10 @@
         <v>36</v>
       </c>
       <c r="B238" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C238" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.35">
@@ -4393,10 +4393,10 @@
         <v>36</v>
       </c>
       <c r="B239" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C239" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.35">
@@ -4404,10 +4404,10 @@
         <v>36</v>
       </c>
       <c r="B240" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C240" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.35">
@@ -4415,10 +4415,10 @@
         <v>36</v>
       </c>
       <c r="B241" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C241" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.35">
@@ -4426,238 +4426,238 @@
         <v>36</v>
       </c>
       <c r="B242" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C242" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
+        <v>326</v>
+      </c>
+      <c r="B243" t="s">
         <v>327</v>
       </c>
-      <c r="B243" t="s">
-        <v>328</v>
-      </c>
       <c r="C243" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B244" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C244" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B245" t="s">
+        <v>329</v>
+      </c>
+      <c r="C245" t="s">
         <v>330</v>
-      </c>
-      <c r="C245" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B246" t="s">
+        <v>331</v>
+      </c>
+      <c r="C246" t="s">
         <v>332</v>
-      </c>
-      <c r="C246" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B247" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C247" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B248" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C248" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B249" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C249" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B250" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C250" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B251" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C251" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B252" t="s">
+        <v>333</v>
+      </c>
+      <c r="C252" t="s">
         <v>334</v>
-      </c>
-      <c r="C252" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B253" t="s">
+        <v>335</v>
+      </c>
+      <c r="C253" t="s">
         <v>336</v>
-      </c>
-      <c r="C253" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B254" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C254" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B255" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C255" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B256" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C256" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B257" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C257" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B258" t="s">
+        <v>340</v>
+      </c>
+      <c r="C258" t="s">
         <v>341</v>
-      </c>
-      <c r="C258" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B259" t="s">
+        <v>342</v>
+      </c>
+      <c r="C259" t="s">
         <v>343</v>
-      </c>
-      <c r="C259" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B260" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C260" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B261" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C261" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B262" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C262" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B263" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C263" t="s">
         <v>11</v>
@@ -4665,76 +4665,76 @@
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B264" t="s">
+        <v>348</v>
+      </c>
+      <c r="C264" t="s">
         <v>349</v>
-      </c>
-      <c r="C264" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B265" t="s">
+        <v>350</v>
+      </c>
+      <c r="C265" t="s">
         <v>351</v>
-      </c>
-      <c r="C265" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B266" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C266" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B267" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C267" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
+        <v>354</v>
+      </c>
+      <c r="B268" t="s">
         <v>355</v>
       </c>
-      <c r="B268" t="s">
-        <v>356</v>
-      </c>
       <c r="C268" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B269" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C269" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B270" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C270" t="s">
         <v>63</v>
@@ -4742,10 +4742,10 @@
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B271" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C271" t="s">
         <v>55</v>
@@ -4753,10 +4753,10 @@
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B272" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C272" t="s">
         <v>51</v>
@@ -4764,208 +4764,208 @@
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B273" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C273" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B274" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C274" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B275" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C275" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
+        <v>363</v>
+      </c>
+      <c r="B276" t="s">
         <v>364</v>
       </c>
-      <c r="B276" t="s">
-        <v>365</v>
-      </c>
       <c r="C276" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B277" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C277" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B278" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C278" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B279" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C279" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B280" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C280" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
+        <v>369</v>
+      </c>
+      <c r="B281" t="s">
         <v>370</v>
       </c>
-      <c r="B281" t="s">
-        <v>371</v>
-      </c>
       <c r="C281" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B282" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C282" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B283" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C283" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B284" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C284" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B285" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C285" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B286" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C286" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B287" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C287" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B288" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C288" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
+        <v>378</v>
+      </c>
+      <c r="B289" t="s">
         <v>379</v>
       </c>
-      <c r="B289" t="s">
-        <v>380</v>
-      </c>
       <c r="C289" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
+        <v>380</v>
+      </c>
+      <c r="B290" t="s">
         <v>381</v>
       </c>
-      <c r="B290" t="s">
-        <v>382</v>
-      </c>
       <c r="C290" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B291" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C291" t="s">
         <v>55</v>
@@ -4973,10 +4973,10 @@
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B292" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C292" t="s">
         <v>51</v>
@@ -4984,10 +4984,10 @@
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B293" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C293" t="s">
         <v>63</v>
@@ -4995,35 +4995,35 @@
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B294" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C294" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B295" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C295" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B296" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C296" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>